<commit_message>
downloaded fastat files done
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\itpgrfa_crop_indicator_code\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7220E603-67D1-4280-B126-B74CAB0A4FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4CD841-3634-462E-BDE6-5BF2F620DB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
@@ -34,12 +34,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>url</t>
   </si>
   <si>
     <t>http://fenixservices.fao.org/faostat/static/bulkdownloads/Production_Crops_E_All_Data.zip</t>
+  </si>
+  <si>
+    <t>http://fenixservices.fao.org/faostat/static/bulkdownloads/Trade_Crops_Livestock_E_All_Data.zip</t>
+  </si>
+  <si>
+    <t>http://fenixservices.fao.org/faostat/static/bulkdownloads/FoodSupply_Crops_E_All_Data.zip</t>
+  </si>
+  <si>
+    <t>http://fenixservices.fao.org/faostat/static/bulkdownloads/Population_E_All_Data.zip</t>
+  </si>
+  <si>
+    <t>http://fenixservices.fao.org/faostat/static/bulkdownloads/Value_of_Production_E_All_Data.zip</t>
+  </si>
+  <si>
+    <t>http://fenixservices.fao.org/faostat/static/bulkdownloads/FoodBalanceSheets_E_All_Data.zip</t>
   </si>
 </sst>
 </file>
@@ -391,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545B1D71-383F-4032-899B-A73C19D2F750}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,6 +427,31 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed the method which merge countries with fao data
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\itpgrfa_crop_indicator_code\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A957CB3-9552-4CA7-9F2A-D13EF65EE73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401A5688-A105-4355-A0D2-E1EB4050D443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
+    <workbookView xWindow="3192" yWindow="2640" windowWidth="19272" windowHeight="8916" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
   <sheets>
-    <sheet name="downloads" sheetId="1" r:id="rId1"/>
-    <sheet name="metrics" sheetId="2" r:id="rId2"/>
+    <sheet name="general" sheetId="3" r:id="rId1"/>
+    <sheet name="downloads" sheetId="1" r:id="rId2"/>
+    <sheet name="metrics" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="227">
   <si>
     <t>url</t>
   </si>
@@ -707,6 +708,15 @@
   </si>
   <si>
     <t>fao</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>fao_encoding</t>
+  </si>
+  <si>
+    <t>ISO-8859-1</t>
   </si>
 </sst>
 </file>
@@ -1057,10 +1067,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811487A-6E7B-4C2E-9752-10E8FCDC87C8}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545B1D71-383F-4032-899B-A73C19D2F750}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B7"/>
     </sheetView>
   </sheetViews>
@@ -1130,7 +1175,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5999D9A-B887-407B-9ED8-3246786298CD}">
   <dimension ref="A1:O161"/>
   <sheetViews>

</xml_diff>

<commit_message>
added method to calculate commodities for weight segregation
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\itpgrfa_crop_indicator_code\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC5E13A-8D26-486F-BC74-E57D0BBEFE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E3209F-A9A9-4647-8115-93093B70861F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="230">
   <si>
     <t>url</t>
   </si>
@@ -720,6 +720,12 @@
   </si>
   <si>
     <t>Production_Crops_E_All_Data</t>
+  </si>
+  <si>
+    <t>fao_production_field</t>
+  </si>
+  <si>
+    <t>Production</t>
   </si>
 </sst>
 </file>
@@ -1082,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811487A-6E7B-4C2E-9752-10E8FCDC87C8}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1116,6 +1122,14 @@
       </c>
       <c r="B3" t="s">
         <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B4" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
calculated values for fao
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\itpgrfa_crop_indicator_code\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E3209F-A9A9-4647-8115-93093B70861F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA648124-01D2-425B-9844-C754B818B1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
+    <workbookView xWindow="5724" yWindow="2748" windowWidth="16944" windowHeight="9612" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="232">
   <si>
     <t>url</t>
   </si>
@@ -726,6 +726,12 @@
   </si>
   <si>
     <t>Production</t>
+  </si>
+  <si>
+    <t>FoodBalanceSheets_E_All_Data</t>
+  </si>
+  <si>
+    <t>fao_special_files</t>
   </si>
 </sst>
 </file>
@@ -1088,15 +1094,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811487A-6E7B-4C2E-9752-10E8FCDC87C8}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1130,6 +1136,14 @@
       </c>
       <c r="B4" t="s">
         <v>229</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
addded counting by countries
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\itpgrfa_crop_indicator_code\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA648124-01D2-425B-9844-C754B818B1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D84B4A-BE18-4D68-8463-0036F3DC0B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5724" yWindow="2748" windowWidth="16944" windowHeight="9612" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="235">
   <si>
     <t>url</t>
   </si>
@@ -732,6 +732,15 @@
   </si>
   <si>
     <t>fao_special_files</t>
+  </si>
+  <si>
+    <t>fao_countries_limit</t>
+  </si>
+  <si>
+    <t>fao_countries_suffix</t>
+  </si>
+  <si>
+    <t>_cumsum</t>
   </si>
 </sst>
 </file>
@@ -1094,10 +1103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811487A-6E7B-4C2E-9752-10E8FCDC87C8}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1144,6 +1153,22 @@
       </c>
       <c r="B5" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B6">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B7" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added google preprocessing data
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\itpgrfa_crop_indicator_code\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6431071-D23E-4030-AEC1-B8B7181FD457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD96AC1A-B453-4C4A-A133-331E6D42CF27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="245">
   <si>
     <t>url</t>
   </si>
@@ -747,6 +747,30 @@
   </si>
   <si>
     <t>Total Population - Both sexes</t>
+  </si>
+  <si>
+    <t>google_file</t>
+  </si>
+  <si>
+    <t>google_sheet</t>
+  </si>
+  <si>
+    <t>Crop List.xlsx</t>
+  </si>
+  <si>
+    <t>GoogleScholar_2019_7_31</t>
+  </si>
+  <si>
+    <t>google_field_crop</t>
+  </si>
+  <si>
+    <t>Common_name_standard</t>
+  </si>
+  <si>
+    <t>google_fields_elements</t>
+  </si>
+  <si>
+    <t>Google citations common name,Google citations genus,Google citations taxon</t>
   </si>
 </sst>
 </file>
@@ -1109,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811487A-6E7B-4C2E-9752-10E8FCDC87C8}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1185,6 +1209,38 @@
         <v>236</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>237</v>
+      </c>
+      <c r="B9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B10" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>241</v>
+      </c>
+      <c r="B11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B12" t="s">
+        <v>244</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1195,7 +1251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545B1D71-383F-4032-899B-A73C19D2F750}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added code to get information from wikipedia
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\itpgrfa_crop_indicator_code\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD96AC1A-B453-4C4A-A133-331E6D42CF27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA88AFE-DF8B-4871-BDF5-005ADC33A20B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="250">
   <si>
     <t>url</t>
   </si>
@@ -771,6 +771,21 @@
   </si>
   <si>
     <t>Google citations common name,Google citations genus,Google citations taxon</t>
+  </si>
+  <si>
+    <t>wikipedia_url</t>
+  </si>
+  <si>
+    <t>https://wikimedia.org/api/rest_v1/metrics/pageviews/per-article/en.wikipedia/all-access/all-agents/</t>
+  </si>
+  <si>
+    <t>wikipedia_timing</t>
+  </si>
+  <si>
+    <t>monthly</t>
+  </si>
+  <si>
+    <t>wikipedia_years</t>
   </si>
 </sst>
 </file>
@@ -1133,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811487A-6E7B-4C2E-9752-10E8FCDC87C8}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1241,9 +1256,36 @@
         <v>244</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>247</v>
+      </c>
+      <c r="B14" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>249</v>
+      </c>
+      <c r="B15">
+        <v>2019</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{6B12AD9C-3007-469C-B4F5-178135E8E695}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added fao sow iii data
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\itpgrfa_crop_indicator_code\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA88AFE-DF8B-4871-BDF5-005ADC33A20B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B6598C-8D30-4A82-B7EA-6A4732B57679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="271">
   <si>
     <t>url</t>
   </si>
@@ -786,6 +786,69 @@
   </si>
   <si>
     <t>wikipedia_years</t>
+  </si>
+  <si>
+    <t>genebank_fields</t>
+  </si>
+  <si>
+    <t>genus_count_origin_supply,species_count_origin_supply</t>
+  </si>
+  <si>
+    <t>upov_fields</t>
+  </si>
+  <si>
+    <t>gbif_research_fields</t>
+  </si>
+  <si>
+    <t>genus_count_gbif_research_supply,species_count_gbif_research_supply</t>
+  </si>
+  <si>
+    <t>fao_sow_file</t>
+  </si>
+  <si>
+    <t>fao_sow.csv</t>
+  </si>
+  <si>
+    <t>fao_sow_field_crop</t>
+  </si>
+  <si>
+    <t>crop_list_equivalent</t>
+  </si>
+  <si>
+    <t>Total transfers</t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>fao_sow_field_count</t>
+  </si>
+  <si>
+    <t>Number_of_samples</t>
+  </si>
+  <si>
+    <t>fao_sow_field_filter</t>
+  </si>
+  <si>
+    <t>fao_sow_value_filter</t>
+  </si>
+  <si>
+    <t>fao_sow_field_year</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>fao_sow_years</t>
+  </si>
+  <si>
+    <t>fao_sow_field_recipient</t>
+  </si>
+  <si>
+    <t>recipient_country</t>
+  </si>
+  <si>
+    <t>2015,2016,2017,2018</t>
   </si>
 </sst>
 </file>
@@ -830,9 +893,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1148,16 +1212,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811487A-6E7B-4C2E-9752-10E8FCDC87C8}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1278,6 +1342,94 @@
       </c>
       <c r="B15">
         <v>2019</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>250</v>
+      </c>
+      <c r="B16" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>252</v>
+      </c>
+      <c r="B17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>253</v>
+      </c>
+      <c r="B18" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>255</v>
+      </c>
+      <c r="B19" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>257</v>
+      </c>
+      <c r="B20" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>263</v>
+      </c>
+      <c r="B21" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>264</v>
+      </c>
+      <c r="B22" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>261</v>
+      </c>
+      <c r="B23" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>265</v>
+      </c>
+      <c r="B24" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>267</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>268</v>
+      </c>
+      <c r="B26" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new step in fao for interdependence
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\itpgrfa_crop_indicator_code\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9499979D-8991-422C-89C7-BAF43DA511E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07040482-3182-4EC2-8442-C89455C16A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="3" r:id="rId1"/>
     <sheet name="downloads" sheetId="1" r:id="rId2"/>
     <sheet name="metrics" sheetId="2" r:id="rId3"/>
+    <sheet name="indicator" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2362" uniqueCount="369">
   <si>
     <t>url</t>
   </si>
@@ -882,13 +883,274 @@
   </si>
   <si>
     <t>fao_wiews_value_filter</t>
+  </si>
+  <si>
+    <t>fao_wiews_field_year</t>
+  </si>
+  <si>
+    <t>fao_wiews_years</t>
+  </si>
+  <si>
+    <t>fao_wiews_field_recipient</t>
+  </si>
+  <si>
+    <t>Germplasm_distributions</t>
+  </si>
+  <si>
+    <t>fao_views.csv</t>
+  </si>
+  <si>
+    <t>fao_wiews_fields_elements</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>CropList_equivalent</t>
+  </si>
+  <si>
+    <t>Total_Accs,Total_Samples</t>
+  </si>
+  <si>
+    <t>reporting_year_endyear</t>
+  </si>
+  <si>
+    <t>Provider_country_or_area</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>element</t>
+  </si>
+  <si>
+    <t>Production_Crops_E_All_Data.csv</t>
+  </si>
+  <si>
+    <t>Area harvested</t>
+  </si>
+  <si>
+    <t>Gross Production Value (current thousand US$)</t>
+  </si>
+  <si>
+    <t>Value_of_Production_E_All_Data.csv</t>
+  </si>
+  <si>
+    <t>folder</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Fat supply quantity (g/capita/day)</t>
+  </si>
+  <si>
+    <t>FoodBalanceSheets_E_All_Data.csv</t>
+  </si>
+  <si>
+    <t>Food supply (kcal/capita/day)</t>
+  </si>
+  <si>
+    <t>Food supply quantity (kg/capita/yr)</t>
+  </si>
+  <si>
+    <t>Protein supply quantity (g/capita/day)</t>
+  </si>
+  <si>
+    <t>Export Quantity</t>
+  </si>
+  <si>
+    <t>Export Value</t>
+  </si>
+  <si>
+    <t>Import Quantity</t>
+  </si>
+  <si>
+    <t>Import Value</t>
+  </si>
+  <si>
+    <t>genebank_distributions_treaty</t>
+  </si>
+  <si>
+    <t>equality_of_demand_countcountries_treaty</t>
+  </si>
+  <si>
+    <t>countcountries_germplasm_distributions</t>
+  </si>
+  <si>
+    <t>equality_of_demand_gini_treaty</t>
+  </si>
+  <si>
+    <t>genebank_distributions_fao_wiews_accessions</t>
+  </si>
+  <si>
+    <t>genebank_distributions_fao_wiews_samples</t>
+  </si>
+  <si>
+    <t>digital_sequence_supply_nucleotide</t>
+  </si>
+  <si>
+    <t>digital_sequence_supply_protein</t>
+  </si>
+  <si>
+    <t>digital_sequence_supply_genome</t>
+  </si>
+  <si>
+    <t>digital_sequence_supply_gene</t>
+  </si>
+  <si>
+    <t>backup_genebank_accessions</t>
+  </si>
+  <si>
+    <t>genus_backup_genebank_accessions</t>
+  </si>
+  <si>
+    <t>species_backup_genebank_accessions</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>prefix_year</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>google</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>google.csv</t>
+  </si>
+  <si>
+    <t>Google citations common name</t>
+  </si>
+  <si>
+    <t>Google citations genus</t>
+  </si>
+  <si>
+    <t>Google citations taxon</t>
+  </si>
+  <si>
+    <t>wikipedia</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>wikipedia.csv</t>
+  </si>
+  <si>
+    <t>genus_count</t>
+  </si>
+  <si>
+    <t>common_name_count</t>
+  </si>
+  <si>
+    <t>taxa_count</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>mls_accesions</t>
+  </si>
+  <si>
+    <t>mls_accessions.csv</t>
+  </si>
+  <si>
+    <t>mls_accessions-genus</t>
+  </si>
+  <si>
+    <t>mls_accessions-species</t>
+  </si>
+  <si>
+    <t>mls_institutions</t>
+  </si>
+  <si>
+    <t>mls_institutions.csv</t>
+  </si>
+  <si>
+    <t>mls_institutions_genus</t>
+  </si>
+  <si>
+    <t>mls_institutions_species</t>
+  </si>
+  <si>
+    <t>fao_wiews</t>
+  </si>
+  <si>
+    <t>fao_wiews.csv</t>
+  </si>
+  <si>
+    <t>Total_Accs</t>
+  </si>
+  <si>
+    <t>Total_Samples</t>
+  </si>
+  <si>
+    <t>fao_sow</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>gini_sample_recipients</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>countries_recipients</t>
+  </si>
+  <si>
+    <t>samples</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>upov</t>
+  </si>
+  <si>
+    <t>upov_varietal_release.csv</t>
+  </si>
+  <si>
+    <t>genebank</t>
+  </si>
+  <si>
+    <t>genebank_collection.csv</t>
+  </si>
+  <si>
+    <t>gbif</t>
+  </si>
+  <si>
+    <t>gbif_research_supply.csv</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -900,6 +1162,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1247,13 +1515,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811487A-6E7B-4C2E-9752-10E8FCDC87C8}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="85" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1502,7 +1770,7 @@
         <v>278</v>
       </c>
       <c r="B31" t="s">
-        <v>256</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -1510,7 +1778,7 @@
         <v>279</v>
       </c>
       <c r="B32" t="s">
-        <v>258</v>
+        <v>289</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -1518,7 +1786,7 @@
         <v>280</v>
       </c>
       <c r="B33" t="s">
-        <v>260</v>
+        <v>288</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -1526,39 +1794,39 @@
         <v>281</v>
       </c>
       <c r="B34" t="s">
-        <v>259</v>
+        <v>285</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>261</v>
+        <v>287</v>
       </c>
       <c r="B35" t="s">
-        <v>262</v>
+        <v>290</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>265</v>
+        <v>282</v>
       </c>
       <c r="B36" t="s">
-        <v>266</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>267</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>270</v>
+        <v>283</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2019</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="B38" t="s">
-        <v>269</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -9065,4 +9333,2657 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB36A16C-A3A5-425C-AEEC-CE2F39694284}">
+  <dimension ref="A1:J99"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F1" t="s">
+        <v>296</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E2" t="s">
+        <v>299</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C3" t="s">
+        <v>303</v>
+      </c>
+      <c r="D3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E3" t="s">
+        <v>229</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D4" t="s">
+        <v>301</v>
+      </c>
+      <c r="E4" t="s">
+        <v>300</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C5" t="s">
+        <v>303</v>
+      </c>
+      <c r="D5" t="s">
+        <v>305</v>
+      </c>
+      <c r="E5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C6" t="s">
+        <v>303</v>
+      </c>
+      <c r="D6" t="s">
+        <v>305</v>
+      </c>
+      <c r="E6" t="s">
+        <v>306</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>222</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C7" t="s">
+        <v>303</v>
+      </c>
+      <c r="D7" t="s">
+        <v>305</v>
+      </c>
+      <c r="E7" t="s">
+        <v>307</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C8" t="s">
+        <v>303</v>
+      </c>
+      <c r="D8" t="s">
+        <v>305</v>
+      </c>
+      <c r="E8" t="s">
+        <v>308</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C9" t="s">
+        <v>303</v>
+      </c>
+      <c r="D9" t="s">
+        <v>301</v>
+      </c>
+      <c r="E9" t="s">
+        <v>309</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>222</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C10" t="s">
+        <v>303</v>
+      </c>
+      <c r="D10" t="s">
+        <v>301</v>
+      </c>
+      <c r="E10" t="s">
+        <v>310</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>222</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D11" t="s">
+        <v>301</v>
+      </c>
+      <c r="E11" t="s">
+        <v>311</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>222</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C12" t="s">
+        <v>303</v>
+      </c>
+      <c r="D12" t="s">
+        <v>301</v>
+      </c>
+      <c r="E12" t="s">
+        <v>312</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>222</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C13" t="s">
+        <v>303</v>
+      </c>
+      <c r="D13" t="s">
+        <v>298</v>
+      </c>
+      <c r="E13" t="s">
+        <v>299</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>222</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C14" t="s">
+        <v>303</v>
+      </c>
+      <c r="D14" t="s">
+        <v>298</v>
+      </c>
+      <c r="E14" t="s">
+        <v>229</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>222</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C15" t="s">
+        <v>303</v>
+      </c>
+      <c r="D15" t="s">
+        <v>301</v>
+      </c>
+      <c r="E15" t="s">
+        <v>300</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>222</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C16" t="s">
+        <v>303</v>
+      </c>
+      <c r="D16" t="s">
+        <v>305</v>
+      </c>
+      <c r="E16" t="s">
+        <v>304</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>222</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C17" t="s">
+        <v>303</v>
+      </c>
+      <c r="D17" t="s">
+        <v>305</v>
+      </c>
+      <c r="E17" t="s">
+        <v>306</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>222</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C18" t="s">
+        <v>303</v>
+      </c>
+      <c r="D18" t="s">
+        <v>305</v>
+      </c>
+      <c r="E18" t="s">
+        <v>307</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>222</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C19" t="s">
+        <v>303</v>
+      </c>
+      <c r="D19" t="s">
+        <v>305</v>
+      </c>
+      <c r="E19" t="s">
+        <v>308</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>222</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C20" t="s">
+        <v>303</v>
+      </c>
+      <c r="D20" t="s">
+        <v>301</v>
+      </c>
+      <c r="E20" t="s">
+        <v>309</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>222</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C21" t="s">
+        <v>303</v>
+      </c>
+      <c r="D21" t="s">
+        <v>301</v>
+      </c>
+      <c r="E21" t="s">
+        <v>310</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>222</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C22" t="s">
+        <v>303</v>
+      </c>
+      <c r="D22" t="s">
+        <v>301</v>
+      </c>
+      <c r="E22" t="s">
+        <v>311</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>222</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C23" t="s">
+        <v>303</v>
+      </c>
+      <c r="D23" t="s">
+        <v>301</v>
+      </c>
+      <c r="E23" t="s">
+        <v>312</v>
+      </c>
+      <c r="F23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>222</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C24" t="s">
+        <v>303</v>
+      </c>
+      <c r="D24" t="s">
+        <v>298</v>
+      </c>
+      <c r="E24" t="s">
+        <v>299</v>
+      </c>
+      <c r="F24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>222</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C25" t="s">
+        <v>303</v>
+      </c>
+      <c r="D25" t="s">
+        <v>298</v>
+      </c>
+      <c r="E25" t="s">
+        <v>229</v>
+      </c>
+      <c r="F25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H25" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>222</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C26" t="s">
+        <v>303</v>
+      </c>
+      <c r="D26" t="s">
+        <v>301</v>
+      </c>
+      <c r="E26" t="s">
+        <v>300</v>
+      </c>
+      <c r="F26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" t="s">
+        <v>46</v>
+      </c>
+      <c r="I26" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>222</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C27" t="s">
+        <v>303</v>
+      </c>
+      <c r="D27" t="s">
+        <v>305</v>
+      </c>
+      <c r="E27" t="s">
+        <v>304</v>
+      </c>
+      <c r="F27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27" t="s">
+        <v>46</v>
+      </c>
+      <c r="I27" t="s">
+        <v>26</v>
+      </c>
+      <c r="J27" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>222</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C28" t="s">
+        <v>303</v>
+      </c>
+      <c r="D28" t="s">
+        <v>305</v>
+      </c>
+      <c r="E28" t="s">
+        <v>306</v>
+      </c>
+      <c r="F28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>222</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C29" t="s">
+        <v>303</v>
+      </c>
+      <c r="D29" t="s">
+        <v>305</v>
+      </c>
+      <c r="E29" t="s">
+        <v>307</v>
+      </c>
+      <c r="F29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" t="s">
+        <v>44</v>
+      </c>
+      <c r="H29" t="s">
+        <v>49</v>
+      </c>
+      <c r="I29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J29" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>222</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C30" t="s">
+        <v>303</v>
+      </c>
+      <c r="D30" t="s">
+        <v>305</v>
+      </c>
+      <c r="E30" t="s">
+        <v>308</v>
+      </c>
+      <c r="F30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" t="s">
+        <v>44</v>
+      </c>
+      <c r="H30" t="s">
+        <v>49</v>
+      </c>
+      <c r="I30" t="s">
+        <v>32</v>
+      </c>
+      <c r="J30" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>222</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C31" t="s">
+        <v>303</v>
+      </c>
+      <c r="D31" t="s">
+        <v>301</v>
+      </c>
+      <c r="E31" t="s">
+        <v>309</v>
+      </c>
+      <c r="F31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" t="s">
+        <v>44</v>
+      </c>
+      <c r="H31" t="s">
+        <v>51</v>
+      </c>
+      <c r="I31" t="s">
+        <v>35</v>
+      </c>
+      <c r="J31" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>222</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C32" t="s">
+        <v>303</v>
+      </c>
+      <c r="D32" t="s">
+        <v>301</v>
+      </c>
+      <c r="E32" t="s">
+        <v>310</v>
+      </c>
+      <c r="F32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" t="s">
+        <v>44</v>
+      </c>
+      <c r="H32" t="s">
+        <v>51</v>
+      </c>
+      <c r="I32" t="s">
+        <v>36</v>
+      </c>
+      <c r="J32" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>222</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C33" t="s">
+        <v>303</v>
+      </c>
+      <c r="D33" t="s">
+        <v>301</v>
+      </c>
+      <c r="E33" t="s">
+        <v>311</v>
+      </c>
+      <c r="F33" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H33" t="s">
+        <v>51</v>
+      </c>
+      <c r="I33" t="s">
+        <v>38</v>
+      </c>
+      <c r="J33" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>222</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C34" t="s">
+        <v>303</v>
+      </c>
+      <c r="D34" t="s">
+        <v>301</v>
+      </c>
+      <c r="E34" t="s">
+        <v>312</v>
+      </c>
+      <c r="F34" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" t="s">
+        <v>44</v>
+      </c>
+      <c r="H34" t="s">
+        <v>51</v>
+      </c>
+      <c r="I34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J34" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" t="s">
+        <v>52</v>
+      </c>
+      <c r="H35" t="s">
+        <v>53</v>
+      </c>
+      <c r="I35" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" t="s">
+        <v>52</v>
+      </c>
+      <c r="H36" t="s">
+        <v>53</v>
+      </c>
+      <c r="I36" t="s">
+        <v>23</v>
+      </c>
+      <c r="J36" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F37" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" t="s">
+        <v>52</v>
+      </c>
+      <c r="H37" t="s">
+        <v>53</v>
+      </c>
+      <c r="I37" t="s">
+        <v>25</v>
+      </c>
+      <c r="J37" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" t="s">
+        <v>53</v>
+      </c>
+      <c r="I38" t="s">
+        <v>26</v>
+      </c>
+      <c r="J38" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F39" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" t="s">
+        <v>52</v>
+      </c>
+      <c r="H39" t="s">
+        <v>59</v>
+      </c>
+      <c r="I39" t="s">
+        <v>28</v>
+      </c>
+      <c r="J39" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F40" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" t="s">
+        <v>52</v>
+      </c>
+      <c r="H40" t="s">
+        <v>59</v>
+      </c>
+      <c r="I40" t="s">
+        <v>30</v>
+      </c>
+      <c r="J40" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" t="s">
+        <v>52</v>
+      </c>
+      <c r="H41" t="s">
+        <v>59</v>
+      </c>
+      <c r="I41" t="s">
+        <v>32</v>
+      </c>
+      <c r="J41" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F42" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" t="s">
+        <v>52</v>
+      </c>
+      <c r="H42" t="s">
+        <v>63</v>
+      </c>
+      <c r="I42" t="s">
+        <v>35</v>
+      </c>
+      <c r="J42" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F43" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" t="s">
+        <v>52</v>
+      </c>
+      <c r="H43" t="s">
+        <v>63</v>
+      </c>
+      <c r="I43" t="s">
+        <v>36</v>
+      </c>
+      <c r="J43" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F44" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" t="s">
+        <v>52</v>
+      </c>
+      <c r="H44" t="s">
+        <v>63</v>
+      </c>
+      <c r="I44" t="s">
+        <v>38</v>
+      </c>
+      <c r="J44" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F45" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" t="s">
+        <v>52</v>
+      </c>
+      <c r="H45" t="s">
+        <v>63</v>
+      </c>
+      <c r="I45" t="s">
+        <v>39</v>
+      </c>
+      <c r="J45" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>330</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C46" t="s">
+        <v>303</v>
+      </c>
+      <c r="D46" t="s">
+        <v>332</v>
+      </c>
+      <c r="E46" t="s">
+        <v>333</v>
+      </c>
+      <c r="F46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" t="s">
+        <v>68</v>
+      </c>
+      <c r="H46" t="s">
+        <v>69</v>
+      </c>
+      <c r="I46" t="s">
+        <v>70</v>
+      </c>
+      <c r="J46" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>330</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C47" t="s">
+        <v>303</v>
+      </c>
+      <c r="D47" t="s">
+        <v>332</v>
+      </c>
+      <c r="E47" t="s">
+        <v>334</v>
+      </c>
+      <c r="F47" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" t="s">
+        <v>68</v>
+      </c>
+      <c r="H47" t="s">
+        <v>69</v>
+      </c>
+      <c r="I47" t="s">
+        <v>71</v>
+      </c>
+      <c r="J47" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>330</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C48" t="s">
+        <v>303</v>
+      </c>
+      <c r="D48" t="s">
+        <v>332</v>
+      </c>
+      <c r="E48" t="s">
+        <v>335</v>
+      </c>
+      <c r="F48" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" t="s">
+        <v>68</v>
+      </c>
+      <c r="H48" t="s">
+        <v>69</v>
+      </c>
+      <c r="I48" t="s">
+        <v>72</v>
+      </c>
+      <c r="J48" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>336</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C49" t="s">
+        <v>337</v>
+      </c>
+      <c r="D49" t="s">
+        <v>338</v>
+      </c>
+      <c r="E49" t="s">
+        <v>340</v>
+      </c>
+      <c r="F49" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" t="s">
+        <v>73</v>
+      </c>
+      <c r="H49" t="s">
+        <v>74</v>
+      </c>
+      <c r="I49" t="s">
+        <v>70</v>
+      </c>
+      <c r="J49" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>336</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C50" t="s">
+        <v>337</v>
+      </c>
+      <c r="D50" t="s">
+        <v>338</v>
+      </c>
+      <c r="E50" t="s">
+        <v>339</v>
+      </c>
+      <c r="F50" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" t="s">
+        <v>73</v>
+      </c>
+      <c r="H50" t="s">
+        <v>74</v>
+      </c>
+      <c r="I50" t="s">
+        <v>71</v>
+      </c>
+      <c r="J50" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>336</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C51" t="s">
+        <v>337</v>
+      </c>
+      <c r="D51" t="s">
+        <v>338</v>
+      </c>
+      <c r="E51" t="s">
+        <v>341</v>
+      </c>
+      <c r="F51" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" t="s">
+        <v>73</v>
+      </c>
+      <c r="H51" t="s">
+        <v>74</v>
+      </c>
+      <c r="I51" t="s">
+        <v>72</v>
+      </c>
+      <c r="J51" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>222</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C52" t="s">
+        <v>303</v>
+      </c>
+      <c r="D52" t="s">
+        <v>298</v>
+      </c>
+      <c r="E52" t="s">
+        <v>299</v>
+      </c>
+      <c r="F52" t="s">
+        <v>75</v>
+      </c>
+      <c r="G52" t="s">
+        <v>17</v>
+      </c>
+      <c r="H52" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" t="s">
+        <v>76</v>
+      </c>
+      <c r="J52" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>222</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C53" t="s">
+        <v>303</v>
+      </c>
+      <c r="D53" t="s">
+        <v>298</v>
+      </c>
+      <c r="E53" t="s">
+        <v>229</v>
+      </c>
+      <c r="F53" t="s">
+        <v>75</v>
+      </c>
+      <c r="G53" t="s">
+        <v>17</v>
+      </c>
+      <c r="H53" t="s">
+        <v>18</v>
+      </c>
+      <c r="I53" t="s">
+        <v>78</v>
+      </c>
+      <c r="J53" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>222</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C54" t="s">
+        <v>303</v>
+      </c>
+      <c r="D54" t="s">
+        <v>301</v>
+      </c>
+      <c r="E54" t="s">
+        <v>300</v>
+      </c>
+      <c r="F54" t="s">
+        <v>75</v>
+      </c>
+      <c r="G54" t="s">
+        <v>17</v>
+      </c>
+      <c r="H54" t="s">
+        <v>18</v>
+      </c>
+      <c r="I54" t="s">
+        <v>79</v>
+      </c>
+      <c r="J54" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>222</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C55" t="s">
+        <v>303</v>
+      </c>
+      <c r="D55" t="s">
+        <v>305</v>
+      </c>
+      <c r="E55" t="s">
+        <v>304</v>
+      </c>
+      <c r="F55" t="s">
+        <v>75</v>
+      </c>
+      <c r="G55" t="s">
+        <v>17</v>
+      </c>
+      <c r="H55" t="s">
+        <v>18</v>
+      </c>
+      <c r="I55" t="s">
+        <v>80</v>
+      </c>
+      <c r="J55" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>222</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C56" t="s">
+        <v>303</v>
+      </c>
+      <c r="D56" t="s">
+        <v>305</v>
+      </c>
+      <c r="E56" t="s">
+        <v>306</v>
+      </c>
+      <c r="F56" t="s">
+        <v>75</v>
+      </c>
+      <c r="G56" t="s">
+        <v>17</v>
+      </c>
+      <c r="H56" t="s">
+        <v>27</v>
+      </c>
+      <c r="I56" t="s">
+        <v>81</v>
+      </c>
+      <c r="J56" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>222</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C57" t="s">
+        <v>303</v>
+      </c>
+      <c r="D57" t="s">
+        <v>305</v>
+      </c>
+      <c r="E57" t="s">
+        <v>307</v>
+      </c>
+      <c r="F57" t="s">
+        <v>75</v>
+      </c>
+      <c r="G57" t="s">
+        <v>17</v>
+      </c>
+      <c r="H57" t="s">
+        <v>27</v>
+      </c>
+      <c r="I57" t="s">
+        <v>82</v>
+      </c>
+      <c r="J57" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>222</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C58" t="s">
+        <v>303</v>
+      </c>
+      <c r="D58" t="s">
+        <v>305</v>
+      </c>
+      <c r="E58" t="s">
+        <v>308</v>
+      </c>
+      <c r="F58" t="s">
+        <v>75</v>
+      </c>
+      <c r="G58" t="s">
+        <v>17</v>
+      </c>
+      <c r="H58" t="s">
+        <v>27</v>
+      </c>
+      <c r="I58" t="s">
+        <v>83</v>
+      </c>
+      <c r="J58" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>222</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C59" t="s">
+        <v>303</v>
+      </c>
+      <c r="D59" t="s">
+        <v>301</v>
+      </c>
+      <c r="E59" t="s">
+        <v>309</v>
+      </c>
+      <c r="F59" t="s">
+        <v>75</v>
+      </c>
+      <c r="G59" t="s">
+        <v>17</v>
+      </c>
+      <c r="H59" t="s">
+        <v>34</v>
+      </c>
+      <c r="I59" t="s">
+        <v>84</v>
+      </c>
+      <c r="J59" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>222</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C60" t="s">
+        <v>303</v>
+      </c>
+      <c r="D60" t="s">
+        <v>301</v>
+      </c>
+      <c r="E60" t="s">
+        <v>310</v>
+      </c>
+      <c r="F60" t="s">
+        <v>75</v>
+      </c>
+      <c r="G60" t="s">
+        <v>17</v>
+      </c>
+      <c r="H60" t="s">
+        <v>34</v>
+      </c>
+      <c r="I60" t="s">
+        <v>85</v>
+      </c>
+      <c r="J60" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>222</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C61" t="s">
+        <v>303</v>
+      </c>
+      <c r="D61" t="s">
+        <v>301</v>
+      </c>
+      <c r="E61" t="s">
+        <v>311</v>
+      </c>
+      <c r="F61" t="s">
+        <v>75</v>
+      </c>
+      <c r="G61" t="s">
+        <v>17</v>
+      </c>
+      <c r="H61" t="s">
+        <v>34</v>
+      </c>
+      <c r="I61" t="s">
+        <v>86</v>
+      </c>
+      <c r="J61" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>222</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C62" t="s">
+        <v>303</v>
+      </c>
+      <c r="D62" t="s">
+        <v>301</v>
+      </c>
+      <c r="E62" t="s">
+        <v>312</v>
+      </c>
+      <c r="F62" t="s">
+        <v>75</v>
+      </c>
+      <c r="G62" t="s">
+        <v>17</v>
+      </c>
+      <c r="H62" t="s">
+        <v>34</v>
+      </c>
+      <c r="I62" t="s">
+        <v>87</v>
+      </c>
+      <c r="J62" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F63" t="s">
+        <v>75</v>
+      </c>
+      <c r="G63" t="s">
+        <v>52</v>
+      </c>
+      <c r="H63" t="s">
+        <v>18</v>
+      </c>
+      <c r="I63" t="s">
+        <v>76</v>
+      </c>
+      <c r="J63" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F64" t="s">
+        <v>75</v>
+      </c>
+      <c r="G64" t="s">
+        <v>52</v>
+      </c>
+      <c r="H64" t="s">
+        <v>18</v>
+      </c>
+      <c r="I64" t="s">
+        <v>78</v>
+      </c>
+      <c r="J64" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F65" t="s">
+        <v>75</v>
+      </c>
+      <c r="G65" t="s">
+        <v>52</v>
+      </c>
+      <c r="H65" t="s">
+        <v>18</v>
+      </c>
+      <c r="I65" t="s">
+        <v>79</v>
+      </c>
+      <c r="J65" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F66" t="s">
+        <v>75</v>
+      </c>
+      <c r="G66" t="s">
+        <v>52</v>
+      </c>
+      <c r="H66" t="s">
+        <v>18</v>
+      </c>
+      <c r="I66" t="s">
+        <v>80</v>
+      </c>
+      <c r="J66" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F67" t="s">
+        <v>75</v>
+      </c>
+      <c r="G67" t="s">
+        <v>52</v>
+      </c>
+      <c r="H67" t="s">
+        <v>27</v>
+      </c>
+      <c r="I67" t="s">
+        <v>81</v>
+      </c>
+      <c r="J67" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F68" t="s">
+        <v>75</v>
+      </c>
+      <c r="G68" t="s">
+        <v>52</v>
+      </c>
+      <c r="H68" t="s">
+        <v>27</v>
+      </c>
+      <c r="I68" t="s">
+        <v>82</v>
+      </c>
+      <c r="J68" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F69" t="s">
+        <v>75</v>
+      </c>
+      <c r="G69" t="s">
+        <v>52</v>
+      </c>
+      <c r="H69" t="s">
+        <v>27</v>
+      </c>
+      <c r="I69" t="s">
+        <v>83</v>
+      </c>
+      <c r="J69" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F70" t="s">
+        <v>75</v>
+      </c>
+      <c r="G70" t="s">
+        <v>52</v>
+      </c>
+      <c r="H70" t="s">
+        <v>34</v>
+      </c>
+      <c r="I70" t="s">
+        <v>84</v>
+      </c>
+      <c r="J70" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F71" t="s">
+        <v>75</v>
+      </c>
+      <c r="G71" t="s">
+        <v>52</v>
+      </c>
+      <c r="H71" t="s">
+        <v>34</v>
+      </c>
+      <c r="I71" t="s">
+        <v>85</v>
+      </c>
+      <c r="J71" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F72" t="s">
+        <v>75</v>
+      </c>
+      <c r="G72" t="s">
+        <v>52</v>
+      </c>
+      <c r="H72" t="s">
+        <v>34</v>
+      </c>
+      <c r="I72" t="s">
+        <v>86</v>
+      </c>
+      <c r="J72" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F73" t="s">
+        <v>75</v>
+      </c>
+      <c r="G73" t="s">
+        <v>52</v>
+      </c>
+      <c r="H73" t="s">
+        <v>34</v>
+      </c>
+      <c r="I73" t="s">
+        <v>87</v>
+      </c>
+      <c r="J73" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>355</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C74" t="s">
+        <v>303</v>
+      </c>
+      <c r="D74" t="s">
+        <v>256</v>
+      </c>
+      <c r="E74" t="s">
+        <v>360</v>
+      </c>
+      <c r="F74" t="s">
+        <v>88</v>
+      </c>
+      <c r="G74" t="s">
+        <v>313</v>
+      </c>
+      <c r="H74" t="s">
+        <v>313</v>
+      </c>
+      <c r="I74" t="s">
+        <v>93</v>
+      </c>
+      <c r="J74" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>355</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C75" t="s">
+        <v>303</v>
+      </c>
+      <c r="D75" t="s">
+        <v>256</v>
+      </c>
+      <c r="E75" t="s">
+        <v>359</v>
+      </c>
+      <c r="F75" t="s">
+        <v>88</v>
+      </c>
+      <c r="G75" t="s">
+        <v>314</v>
+      </c>
+      <c r="H75" t="s">
+        <v>315</v>
+      </c>
+      <c r="I75" t="s">
+        <v>315</v>
+      </c>
+      <c r="J75" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>355</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C76" t="s">
+        <v>303</v>
+      </c>
+      <c r="D76" t="s">
+        <v>256</v>
+      </c>
+      <c r="E76" t="s">
+        <v>357</v>
+      </c>
+      <c r="F76" t="s">
+        <v>88</v>
+      </c>
+      <c r="G76" t="s">
+        <v>316</v>
+      </c>
+      <c r="H76" t="s">
+        <v>95</v>
+      </c>
+      <c r="I76" t="s">
+        <v>96</v>
+      </c>
+      <c r="J76" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>351</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C77" t="s">
+        <v>303</v>
+      </c>
+      <c r="D77" t="s">
+        <v>352</v>
+      </c>
+      <c r="E77" t="s">
+        <v>353</v>
+      </c>
+      <c r="F77" t="s">
+        <v>88</v>
+      </c>
+      <c r="G77" t="s">
+        <v>90</v>
+      </c>
+      <c r="H77" t="s">
+        <v>317</v>
+      </c>
+      <c r="I77" t="s">
+        <v>317</v>
+      </c>
+      <c r="J77" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>351</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C78" t="s">
+        <v>303</v>
+      </c>
+      <c r="D78" t="s">
+        <v>352</v>
+      </c>
+      <c r="E78" t="s">
+        <v>354</v>
+      </c>
+      <c r="F78" t="s">
+        <v>88</v>
+      </c>
+      <c r="G78" t="s">
+        <v>90</v>
+      </c>
+      <c r="H78" t="s">
+        <v>318</v>
+      </c>
+      <c r="I78" t="s">
+        <v>318</v>
+      </c>
+      <c r="J78" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F79" t="s">
+        <v>88</v>
+      </c>
+      <c r="G79" t="s">
+        <v>98</v>
+      </c>
+      <c r="H79" t="s">
+        <v>98</v>
+      </c>
+      <c r="I79" t="s">
+        <v>98</v>
+      </c>
+      <c r="J79" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>362</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C80" t="s">
+        <v>337</v>
+      </c>
+      <c r="D80" t="s">
+        <v>363</v>
+      </c>
+      <c r="E80" t="s">
+        <v>101</v>
+      </c>
+      <c r="F80" t="s">
+        <v>88</v>
+      </c>
+      <c r="G80" t="s">
+        <v>100</v>
+      </c>
+      <c r="H80" t="s">
+        <v>100</v>
+      </c>
+      <c r="I80" t="s">
+        <v>101</v>
+      </c>
+      <c r="J80" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>364</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C81" t="s">
+        <v>337</v>
+      </c>
+      <c r="D81" t="s">
+        <v>365</v>
+      </c>
+      <c r="E81" t="s">
+        <v>107</v>
+      </c>
+      <c r="F81" t="s">
+        <v>104</v>
+      </c>
+      <c r="G81" t="s">
+        <v>105</v>
+      </c>
+      <c r="H81" t="s">
+        <v>106</v>
+      </c>
+      <c r="I81" t="s">
+        <v>107</v>
+      </c>
+      <c r="J81" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>364</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C82" t="s">
+        <v>337</v>
+      </c>
+      <c r="D82" t="s">
+        <v>365</v>
+      </c>
+      <c r="E82" t="s">
+        <v>109</v>
+      </c>
+      <c r="F82" t="s">
+        <v>104</v>
+      </c>
+      <c r="G82" t="s">
+        <v>105</v>
+      </c>
+      <c r="H82" t="s">
+        <v>106</v>
+      </c>
+      <c r="I82" t="s">
+        <v>109</v>
+      </c>
+      <c r="J82" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>343</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C83" t="s">
+        <v>303</v>
+      </c>
+      <c r="D83" t="s">
+        <v>344</v>
+      </c>
+      <c r="E83" t="s">
+        <v>345</v>
+      </c>
+      <c r="F83" t="s">
+        <v>104</v>
+      </c>
+      <c r="G83" t="s">
+        <v>111</v>
+      </c>
+      <c r="H83" t="s">
+        <v>113</v>
+      </c>
+      <c r="I83" t="s">
+        <v>114</v>
+      </c>
+      <c r="J83" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>343</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C84" t="s">
+        <v>303</v>
+      </c>
+      <c r="D84" t="s">
+        <v>344</v>
+      </c>
+      <c r="E84" t="s">
+        <v>346</v>
+      </c>
+      <c r="F84" t="s">
+        <v>104</v>
+      </c>
+      <c r="G84" t="s">
+        <v>111</v>
+      </c>
+      <c r="H84" t="s">
+        <v>113</v>
+      </c>
+      <c r="I84" t="s">
+        <v>115</v>
+      </c>
+      <c r="J84" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>347</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C85" t="s">
+        <v>303</v>
+      </c>
+      <c r="D85" t="s">
+        <v>348</v>
+      </c>
+      <c r="E85" t="s">
+        <v>349</v>
+      </c>
+      <c r="F85" t="s">
+        <v>104</v>
+      </c>
+      <c r="G85" t="s">
+        <v>111</v>
+      </c>
+      <c r="H85" t="s">
+        <v>117</v>
+      </c>
+      <c r="I85" t="s">
+        <v>118</v>
+      </c>
+      <c r="J85" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>347</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C86" t="s">
+        <v>303</v>
+      </c>
+      <c r="D86" t="s">
+        <v>348</v>
+      </c>
+      <c r="E86" t="s">
+        <v>350</v>
+      </c>
+      <c r="F86" t="s">
+        <v>104</v>
+      </c>
+      <c r="G86" t="s">
+        <v>111</v>
+      </c>
+      <c r="H86" t="s">
+        <v>117</v>
+      </c>
+      <c r="I86" t="s">
+        <v>119</v>
+      </c>
+      <c r="J86" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F87" t="s">
+        <v>104</v>
+      </c>
+      <c r="G87" t="s">
+        <v>126</v>
+      </c>
+      <c r="H87" t="s">
+        <v>126</v>
+      </c>
+      <c r="I87" t="s">
+        <v>127</v>
+      </c>
+      <c r="J87" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F88" t="s">
+        <v>104</v>
+      </c>
+      <c r="G88" t="s">
+        <v>126</v>
+      </c>
+      <c r="H88" t="s">
+        <v>126</v>
+      </c>
+      <c r="I88" t="s">
+        <v>128</v>
+      </c>
+      <c r="J88" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F89" t="s">
+        <v>104</v>
+      </c>
+      <c r="G89" t="s">
+        <v>125</v>
+      </c>
+      <c r="H89" t="s">
+        <v>125</v>
+      </c>
+      <c r="I89" t="s">
+        <v>125</v>
+      </c>
+      <c r="J89" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>366</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C90" t="s">
+        <v>337</v>
+      </c>
+      <c r="D90" t="s">
+        <v>367</v>
+      </c>
+      <c r="E90" t="s">
+        <v>122</v>
+      </c>
+      <c r="F90" t="s">
+        <v>104</v>
+      </c>
+      <c r="G90" t="s">
+        <v>120</v>
+      </c>
+      <c r="H90" t="s">
+        <v>121</v>
+      </c>
+      <c r="I90" t="s">
+        <v>122</v>
+      </c>
+      <c r="J90" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>366</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C91" t="s">
+        <v>337</v>
+      </c>
+      <c r="D91" t="s">
+        <v>367</v>
+      </c>
+      <c r="E91" t="s">
+        <v>124</v>
+      </c>
+      <c r="F91" t="s">
+        <v>104</v>
+      </c>
+      <c r="G91" t="s">
+        <v>120</v>
+      </c>
+      <c r="H91" t="s">
+        <v>121</v>
+      </c>
+      <c r="I91" t="s">
+        <v>124</v>
+      </c>
+      <c r="J91" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F92" t="s">
+        <v>104</v>
+      </c>
+      <c r="G92" t="s">
+        <v>129</v>
+      </c>
+      <c r="H92" t="s">
+        <v>129</v>
+      </c>
+      <c r="I92" t="s">
+        <v>319</v>
+      </c>
+      <c r="J92" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F93" t="s">
+        <v>104</v>
+      </c>
+      <c r="G93" t="s">
+        <v>129</v>
+      </c>
+      <c r="H93" t="s">
+        <v>129</v>
+      </c>
+      <c r="I93" t="s">
+        <v>320</v>
+      </c>
+      <c r="J93" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F94" t="s">
+        <v>104</v>
+      </c>
+      <c r="G94" t="s">
+        <v>129</v>
+      </c>
+      <c r="H94" t="s">
+        <v>129</v>
+      </c>
+      <c r="I94" t="s">
+        <v>321</v>
+      </c>
+      <c r="J94" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F95" t="s">
+        <v>104</v>
+      </c>
+      <c r="G95" t="s">
+        <v>129</v>
+      </c>
+      <c r="H95" t="s">
+        <v>129</v>
+      </c>
+      <c r="I95" t="s">
+        <v>322</v>
+      </c>
+      <c r="J95" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F96" t="s">
+        <v>130</v>
+      </c>
+      <c r="G96" t="s">
+        <v>131</v>
+      </c>
+      <c r="H96" t="s">
+        <v>131</v>
+      </c>
+      <c r="I96" t="s">
+        <v>132</v>
+      </c>
+      <c r="J96" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="97" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F97" t="s">
+        <v>130</v>
+      </c>
+      <c r="G97" t="s">
+        <v>131</v>
+      </c>
+      <c r="H97" t="s">
+        <v>131</v>
+      </c>
+      <c r="I97" t="s">
+        <v>133</v>
+      </c>
+      <c r="J97" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="98" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F98" t="s">
+        <v>130</v>
+      </c>
+      <c r="G98" t="s">
+        <v>323</v>
+      </c>
+      <c r="H98" t="s">
+        <v>323</v>
+      </c>
+      <c r="I98" t="s">
+        <v>324</v>
+      </c>
+      <c r="J98" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="99" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F99" t="s">
+        <v>130</v>
+      </c>
+      <c r="G99" t="s">
+        <v>323</v>
+      </c>
+      <c r="H99" t="s">
+        <v>323</v>
+      </c>
+      <c r="I99" t="s">
+        <v>325</v>
+      </c>
+      <c r="J99" t="s">
+        <v>329</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added new steps in indicator until step 03. fixed a bug when create files for fao step 02, now it filters by world
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\itpgrfa_crop_indicator_code\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07040482-3182-4EC2-8442-C89455C16A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11A51C8-0E48-4DE3-A409-9F0242DAAC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
@@ -16,8 +16,11 @@
     <sheet name="general" sheetId="3" r:id="rId1"/>
     <sheet name="downloads" sheetId="1" r:id="rId2"/>
     <sheet name="metrics" sheetId="2" r:id="rId3"/>
-    <sheet name="indicator" sheetId="7" r:id="rId4"/>
+    <sheet name="indicator" sheetId="8" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">indicator!$A$1:$J$99</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2362" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="371">
   <si>
     <t>url</t>
   </si>
@@ -912,9 +915,6 @@
     <t>Total_Accs,Total_Samples</t>
   </si>
   <si>
-    <t>reporting_year_endyear</t>
-  </si>
-  <si>
     <t>Provider_country_or_area</t>
   </si>
   <si>
@@ -1144,13 +1144,22 @@
   </si>
   <si>
     <t>13</t>
+  </si>
+  <si>
+    <t>fill_zero</t>
+  </si>
+  <si>
+    <t>Trade_Crops_Livestock_E_All_Data.csv</t>
+  </si>
+  <si>
+    <t>Reporting_year_endyear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1162,12 +1171,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1810,7 +1813,7 @@
         <v>282</v>
       </c>
       <c r="B36" t="s">
-        <v>291</v>
+        <v>370</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -1826,7 +1829,7 @@
         <v>284</v>
       </c>
       <c r="B38" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -9336,11 +9339,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB36A16C-A3A5-425C-AEEC-CE2F39694284}">
-  <dimension ref="A1:J99"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2D5B62-00C5-4824-8379-4A4BEE02241D}">
+  <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9351,29 +9354,30 @@
     <col min="4" max="4" width="31.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.88671875" customWidth="1"/>
     <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" t="s">
         <v>293</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D1" t="s">
         <v>294</v>
       </c>
-      <c r="C1" t="s">
-        <v>302</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F1" t="s">
         <v>295</v>
-      </c>
-      <c r="E1" t="s">
-        <v>297</v>
-      </c>
-      <c r="F1" t="s">
-        <v>296</v>
       </c>
       <c r="G1" t="s">
         <v>7</v>
@@ -9385,24 +9389,27 @@
         <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+      <c r="K1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>222</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E2" t="s">
         <v>303</v>
-      </c>
-      <c r="D2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E2" t="s">
-        <v>299</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -9417,24 +9424,24 @@
         <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>222</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D3" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="E3" t="s">
-        <v>229</v>
+        <v>305</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -9449,24 +9456,24 @@
         <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>222</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D4" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="E4" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
@@ -9481,24 +9488,24 @@
         <v>25</v>
       </c>
       <c r="J4" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>222</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E5" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
@@ -9513,24 +9520,24 @@
         <v>26</v>
       </c>
       <c r="J5" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>222</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D6" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E6" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
@@ -9545,24 +9552,24 @@
         <v>28</v>
       </c>
       <c r="J6" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>222</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D7" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E7" t="s">
-        <v>307</v>
+        <v>229</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
@@ -9577,24 +9584,24 @@
         <v>30</v>
       </c>
       <c r="J7" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>222</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E8" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
@@ -9609,24 +9616,24 @@
         <v>32</v>
       </c>
       <c r="J8" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>222</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D9" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
       <c r="E9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
@@ -9641,24 +9648,24 @@
         <v>35</v>
       </c>
       <c r="J9" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>222</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D10" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
       <c r="E10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F10" t="s">
         <v>16</v>
@@ -9673,24 +9680,24 @@
         <v>36</v>
       </c>
       <c r="J10" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>222</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D11" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
       <c r="E11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F11" t="s">
         <v>16</v>
@@ -9705,24 +9712,24 @@
         <v>38</v>
       </c>
       <c r="J11" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>222</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D12" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
       <c r="E12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
@@ -9737,24 +9744,24 @@
         <v>39</v>
       </c>
       <c r="J12" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>222</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C13" t="s">
+        <v>302</v>
+      </c>
+      <c r="D13" t="s">
+        <v>304</v>
+      </c>
+      <c r="E13" t="s">
         <v>303</v>
-      </c>
-      <c r="D13" t="s">
-        <v>298</v>
-      </c>
-      <c r="E13" t="s">
-        <v>299</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
@@ -9769,21 +9776,21 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>222</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D14" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="E14" t="s">
-        <v>229</v>
+        <v>305</v>
       </c>
       <c r="F14" t="s">
         <v>16</v>
@@ -9798,21 +9805,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>222</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D15" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="E15" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="F15" t="s">
         <v>16</v>
@@ -9827,21 +9834,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>222</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C16" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E16" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="F16" t="s">
         <v>16</v>
@@ -9861,16 +9868,16 @@
         <v>222</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D17" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E17" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="F17" t="s">
         <v>16</v>
@@ -9890,16 +9897,16 @@
         <v>222</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D18" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E18" t="s">
-        <v>307</v>
+        <v>229</v>
       </c>
       <c r="F18" t="s">
         <v>16</v>
@@ -9919,16 +9926,16 @@
         <v>222</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D19" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E19" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="F19" t="s">
         <v>16</v>
@@ -9948,16 +9955,16 @@
         <v>222</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C20" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D20" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
       <c r="E20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F20" t="s">
         <v>16</v>
@@ -9977,16 +9984,16 @@
         <v>222</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C21" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D21" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
       <c r="E21" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F21" t="s">
         <v>16</v>
@@ -10006,16 +10013,16 @@
         <v>222</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D22" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
       <c r="E22" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F22" t="s">
         <v>16</v>
@@ -10035,16 +10042,16 @@
         <v>222</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C23" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D23" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
       <c r="E23" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F23" t="s">
         <v>16</v>
@@ -10064,16 +10071,16 @@
         <v>222</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C24" t="s">
+        <v>302</v>
+      </c>
+      <c r="D24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E24" t="s">
         <v>303</v>
-      </c>
-      <c r="D24" t="s">
-        <v>298</v>
-      </c>
-      <c r="E24" t="s">
-        <v>299</v>
       </c>
       <c r="F24" t="s">
         <v>16</v>
@@ -10088,7 +10095,7 @@
         <v>19</v>
       </c>
       <c r="J24" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -10096,16 +10103,16 @@
         <v>222</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C25" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D25" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="E25" t="s">
-        <v>229</v>
+        <v>305</v>
       </c>
       <c r="F25" t="s">
         <v>16</v>
@@ -10120,7 +10127,7 @@
         <v>23</v>
       </c>
       <c r="J25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -10128,16 +10135,16 @@
         <v>222</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D26" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="E26" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="F26" t="s">
         <v>16</v>
@@ -10152,7 +10159,7 @@
         <v>25</v>
       </c>
       <c r="J26" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -10160,16 +10167,16 @@
         <v>222</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C27" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D27" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E27" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="F27" t="s">
         <v>16</v>
@@ -10184,7 +10191,7 @@
         <v>26</v>
       </c>
       <c r="J27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -10192,16 +10199,16 @@
         <v>222</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D28" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E28" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="F28" t="s">
         <v>16</v>
@@ -10216,7 +10223,7 @@
         <v>28</v>
       </c>
       <c r="J28" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -10224,16 +10231,16 @@
         <v>222</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C29" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D29" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E29" t="s">
-        <v>307</v>
+        <v>229</v>
       </c>
       <c r="F29" t="s">
         <v>16</v>
@@ -10248,7 +10255,7 @@
         <v>30</v>
       </c>
       <c r="J29" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -10256,16 +10263,16 @@
         <v>222</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D30" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E30" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="F30" t="s">
         <v>16</v>
@@ -10280,7 +10287,7 @@
         <v>32</v>
       </c>
       <c r="J30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -10288,16 +10295,16 @@
         <v>222</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C31" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D31" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
       <c r="E31" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F31" t="s">
         <v>16</v>
@@ -10312,7 +10319,7 @@
         <v>35</v>
       </c>
       <c r="J31" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -10320,16 +10327,16 @@
         <v>222</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C32" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D32" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
       <c r="E32" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F32" t="s">
         <v>16</v>
@@ -10344,7 +10351,7 @@
         <v>36</v>
       </c>
       <c r="J32" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -10352,16 +10359,16 @@
         <v>222</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D33" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
       <c r="E33" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F33" t="s">
         <v>16</v>
@@ -10376,7 +10383,7 @@
         <v>38</v>
       </c>
       <c r="J33" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
@@ -10384,16 +10391,16 @@
         <v>222</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D34" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
       <c r="E34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F34" t="s">
         <v>16</v>
@@ -10408,7 +10415,7 @@
         <v>39</v>
       </c>
       <c r="J34" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
@@ -10425,7 +10432,7 @@
         <v>19</v>
       </c>
       <c r="J35" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -10442,7 +10449,7 @@
         <v>23</v>
       </c>
       <c r="J36" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -10459,7 +10466,7 @@
         <v>25</v>
       </c>
       <c r="J37" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -10476,7 +10483,7 @@
         <v>26</v>
       </c>
       <c r="J38" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
@@ -10493,7 +10500,7 @@
         <v>28</v>
       </c>
       <c r="J39" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
@@ -10510,7 +10517,7 @@
         <v>30</v>
       </c>
       <c r="J40" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
@@ -10527,7 +10534,7 @@
         <v>32</v>
       </c>
       <c r="J41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -10544,7 +10551,7 @@
         <v>35</v>
       </c>
       <c r="J42" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -10561,7 +10568,7 @@
         <v>36</v>
       </c>
       <c r="J43" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
@@ -10578,7 +10585,7 @@
         <v>38</v>
       </c>
       <c r="J44" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
@@ -10595,24 +10602,24 @@
         <v>39</v>
       </c>
       <c r="J45" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>329</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" t="s">
+        <v>302</v>
+      </c>
+      <c r="D46" t="s">
         <v>331</v>
       </c>
-      <c r="C46" t="s">
-        <v>303</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>332</v>
-      </c>
-      <c r="E46" t="s">
-        <v>333</v>
       </c>
       <c r="F46" t="s">
         <v>16</v>
@@ -10627,24 +10634,24 @@
         <v>70</v>
       </c>
       <c r="J46" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>329</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" t="s">
+        <v>302</v>
+      </c>
+      <c r="D47" t="s">
         <v>331</v>
       </c>
-      <c r="C47" t="s">
-        <v>303</v>
-      </c>
-      <c r="D47" t="s">
-        <v>332</v>
-      </c>
       <c r="E47" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F47" t="s">
         <v>16</v>
@@ -10659,24 +10666,24 @@
         <v>71</v>
       </c>
       <c r="J47" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>329</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" t="s">
+        <v>302</v>
+      </c>
+      <c r="D48" t="s">
         <v>331</v>
       </c>
-      <c r="C48" t="s">
-        <v>303</v>
-      </c>
-      <c r="D48" t="s">
-        <v>332</v>
-      </c>
       <c r="E48" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F48" t="s">
         <v>16</v>
@@ -10691,24 +10698,24 @@
         <v>72</v>
       </c>
       <c r="J48" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>335</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C49" t="s">
         <v>336</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>337</v>
       </c>
-      <c r="D49" t="s">
-        <v>338</v>
-      </c>
       <c r="E49" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F49" t="s">
         <v>16</v>
@@ -10723,24 +10730,24 @@
         <v>70</v>
       </c>
       <c r="J49" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>335</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C50" t="s">
         <v>336</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>337</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>338</v>
-      </c>
-      <c r="E50" t="s">
-        <v>339</v>
       </c>
       <c r="F50" t="s">
         <v>16</v>
@@ -10755,24 +10762,24 @@
         <v>71</v>
       </c>
       <c r="J50" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>335</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C51" t="s">
         <v>336</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>337</v>
       </c>
-      <c r="D51" t="s">
-        <v>338</v>
-      </c>
       <c r="E51" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F51" t="s">
         <v>16</v>
@@ -10787,7 +10794,7 @@
         <v>72</v>
       </c>
       <c r="J51" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
@@ -10795,16 +10802,16 @@
         <v>222</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C52" t="s">
+        <v>302</v>
+      </c>
+      <c r="D52" t="s">
+        <v>304</v>
+      </c>
+      <c r="E52" t="s">
         <v>303</v>
-      </c>
-      <c r="D52" t="s">
-        <v>298</v>
-      </c>
-      <c r="E52" t="s">
-        <v>299</v>
       </c>
       <c r="F52" t="s">
         <v>75</v>
@@ -10819,7 +10826,7 @@
         <v>76</v>
       </c>
       <c r="J52" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -10827,16 +10834,16 @@
         <v>222</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C53" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D53" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="E53" t="s">
-        <v>229</v>
+        <v>305</v>
       </c>
       <c r="F53" t="s">
         <v>75</v>
@@ -10851,7 +10858,7 @@
         <v>78</v>
       </c>
       <c r="J53" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
@@ -10859,16 +10866,16 @@
         <v>222</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C54" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D54" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="E54" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="F54" t="s">
         <v>75</v>
@@ -10883,7 +10890,7 @@
         <v>79</v>
       </c>
       <c r="J54" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
@@ -10891,16 +10898,16 @@
         <v>222</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C55" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D55" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E55" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="F55" t="s">
         <v>75</v>
@@ -10915,7 +10922,7 @@
         <v>80</v>
       </c>
       <c r="J55" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
@@ -10923,16 +10930,16 @@
         <v>222</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C56" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D56" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E56" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="F56" t="s">
         <v>75</v>
@@ -10947,7 +10954,7 @@
         <v>81</v>
       </c>
       <c r="J56" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
@@ -10955,16 +10962,16 @@
         <v>222</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C57" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D57" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E57" t="s">
-        <v>307</v>
+        <v>229</v>
       </c>
       <c r="F57" t="s">
         <v>75</v>
@@ -10976,10 +10983,10 @@
         <v>27</v>
       </c>
       <c r="I57" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J57" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
@@ -10987,16 +10994,16 @@
         <v>222</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C58" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D58" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E58" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="F58" t="s">
         <v>75</v>
@@ -11008,10 +11015,10 @@
         <v>27</v>
       </c>
       <c r="I58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J58" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
@@ -11019,16 +11026,16 @@
         <v>222</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C59" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D59" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
       <c r="E59" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F59" t="s">
         <v>75</v>
@@ -11043,7 +11050,7 @@
         <v>84</v>
       </c>
       <c r="J59" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
@@ -11051,16 +11058,16 @@
         <v>222</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C60" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D60" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
       <c r="E60" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F60" t="s">
         <v>75</v>
@@ -11075,7 +11082,7 @@
         <v>85</v>
       </c>
       <c r="J60" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
@@ -11083,16 +11090,16 @@
         <v>222</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C61" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D61" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
       <c r="E61" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F61" t="s">
         <v>75</v>
@@ -11107,7 +11114,7 @@
         <v>86</v>
       </c>
       <c r="J61" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
@@ -11115,16 +11122,16 @@
         <v>222</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C62" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D62" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
       <c r="E62" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F62" t="s">
         <v>75</v>
@@ -11139,7 +11146,7 @@
         <v>87</v>
       </c>
       <c r="J62" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
@@ -11156,7 +11163,7 @@
         <v>76</v>
       </c>
       <c r="J63" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
@@ -11173,7 +11180,7 @@
         <v>78</v>
       </c>
       <c r="J64" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
@@ -11190,7 +11197,7 @@
         <v>79</v>
       </c>
       <c r="J65" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
@@ -11207,7 +11214,7 @@
         <v>80</v>
       </c>
       <c r="J66" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
@@ -11224,7 +11231,7 @@
         <v>81</v>
       </c>
       <c r="J67" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
@@ -11241,7 +11248,7 @@
         <v>82</v>
       </c>
       <c r="J68" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
@@ -11258,7 +11265,7 @@
         <v>83</v>
       </c>
       <c r="J69" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
@@ -11275,7 +11282,7 @@
         <v>84</v>
       </c>
       <c r="J70" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
@@ -11292,7 +11299,7 @@
         <v>85</v>
       </c>
       <c r="J71" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
@@ -11309,7 +11316,7 @@
         <v>86</v>
       </c>
       <c r="J72" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
@@ -11326,94 +11333,94 @@
         <v>87</v>
       </c>
       <c r="J73" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C74" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D74" t="s">
         <v>256</v>
       </c>
       <c r="E74" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F74" t="s">
         <v>88</v>
       </c>
       <c r="G74" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H74" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I74" t="s">
         <v>93</v>
       </c>
       <c r="J74" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C75" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D75" t="s">
         <v>256</v>
       </c>
       <c r="E75" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F75" t="s">
         <v>88</v>
       </c>
       <c r="G75" t="s">
+        <v>313</v>
+      </c>
+      <c r="H75" t="s">
         <v>314</v>
       </c>
-      <c r="H75" t="s">
-        <v>315</v>
-      </c>
       <c r="I75" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J75" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>354</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>356</v>
-      </c>
       <c r="C76" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D76" t="s">
         <v>256</v>
       </c>
       <c r="E76" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F76" t="s">
         <v>88</v>
       </c>
       <c r="G76" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H76" t="s">
         <v>95</v>
@@ -11422,24 +11429,24 @@
         <v>96</v>
       </c>
       <c r="J76" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>350</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C77" t="s">
+        <v>302</v>
+      </c>
+      <c r="D77" t="s">
         <v>351</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C77" t="s">
-        <v>303</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>352</v>
-      </c>
-      <c r="E77" t="s">
-        <v>353</v>
       </c>
       <c r="F77" t="s">
         <v>88</v>
@@ -11448,30 +11455,30 @@
         <v>90</v>
       </c>
       <c r="H77" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I77" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J77" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
+        <v>350</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C78" t="s">
+        <v>302</v>
+      </c>
+      <c r="D78" t="s">
         <v>351</v>
       </c>
-      <c r="B78" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C78" t="s">
-        <v>303</v>
-      </c>
-      <c r="D78" t="s">
-        <v>352</v>
-      </c>
       <c r="E78" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F78" t="s">
         <v>88</v>
@@ -11480,13 +11487,13 @@
         <v>90</v>
       </c>
       <c r="H78" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I78" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J78" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
@@ -11503,21 +11510,21 @@
         <v>98</v>
       </c>
       <c r="J79" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>361</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C80" t="s">
+        <v>336</v>
+      </c>
+      <c r="D80" t="s">
         <v>362</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C80" t="s">
-        <v>337</v>
-      </c>
-      <c r="D80" t="s">
-        <v>363</v>
       </c>
       <c r="E80" t="s">
         <v>101</v>
@@ -11535,21 +11542,21 @@
         <v>101</v>
       </c>
       <c r="J80" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>363</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C81" t="s">
+        <v>336</v>
+      </c>
+      <c r="D81" t="s">
         <v>364</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C81" t="s">
-        <v>337</v>
-      </c>
-      <c r="D81" t="s">
-        <v>365</v>
       </c>
       <c r="E81" t="s">
         <v>107</v>
@@ -11567,21 +11574,21 @@
         <v>107</v>
       </c>
       <c r="J81" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
+        <v>363</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C82" t="s">
+        <v>336</v>
+      </c>
+      <c r="D82" t="s">
         <v>364</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C82" t="s">
-        <v>337</v>
-      </c>
-      <c r="D82" t="s">
-        <v>365</v>
       </c>
       <c r="E82" t="s">
         <v>109</v>
@@ -11599,24 +11606,24 @@
         <v>109</v>
       </c>
       <c r="J82" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
+        <v>342</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C83" t="s">
+        <v>302</v>
+      </c>
+      <c r="D83" t="s">
         <v>343</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C83" t="s">
-        <v>303</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>344</v>
-      </c>
-      <c r="E83" t="s">
-        <v>345</v>
       </c>
       <c r="F83" t="s">
         <v>104</v>
@@ -11631,24 +11638,24 @@
         <v>114</v>
       </c>
       <c r="J83" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
+        <v>342</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C84" t="s">
+        <v>302</v>
+      </c>
+      <c r="D84" t="s">
         <v>343</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C84" t="s">
-        <v>303</v>
-      </c>
-      <c r="D84" t="s">
-        <v>344</v>
-      </c>
       <c r="E84" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F84" t="s">
         <v>104</v>
@@ -11663,24 +11670,24 @@
         <v>115</v>
       </c>
       <c r="J84" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
+        <v>346</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C85" t="s">
+        <v>302</v>
+      </c>
+      <c r="D85" t="s">
         <v>347</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C85" t="s">
-        <v>303</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>348</v>
-      </c>
-      <c r="E85" t="s">
-        <v>349</v>
       </c>
       <c r="F85" t="s">
         <v>104</v>
@@ -11695,24 +11702,24 @@
         <v>118</v>
       </c>
       <c r="J85" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
+        <v>346</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C86" t="s">
+        <v>302</v>
+      </c>
+      <c r="D86" t="s">
         <v>347</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C86" t="s">
-        <v>303</v>
-      </c>
-      <c r="D86" t="s">
-        <v>348</v>
-      </c>
       <c r="E86" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F86" t="s">
         <v>104</v>
@@ -11727,7 +11734,7 @@
         <v>119</v>
       </c>
       <c r="J86" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
@@ -11744,7 +11751,7 @@
         <v>127</v>
       </c>
       <c r="J87" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
@@ -11761,7 +11768,7 @@
         <v>128</v>
       </c>
       <c r="J88" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
@@ -11778,21 +11785,21 @@
         <v>125</v>
       </c>
       <c r="J89" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
+        <v>365</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C90" t="s">
+        <v>336</v>
+      </c>
+      <c r="D90" t="s">
         <v>366</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C90" t="s">
-        <v>337</v>
-      </c>
-      <c r="D90" t="s">
-        <v>367</v>
       </c>
       <c r="E90" t="s">
         <v>122</v>
@@ -11810,21 +11817,21 @@
         <v>122</v>
       </c>
       <c r="J90" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
+        <v>365</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C91" t="s">
+        <v>336</v>
+      </c>
+      <c r="D91" t="s">
         <v>366</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C91" t="s">
-        <v>337</v>
-      </c>
-      <c r="D91" t="s">
-        <v>367</v>
       </c>
       <c r="E91" t="s">
         <v>124</v>
@@ -11842,7 +11849,7 @@
         <v>124</v>
       </c>
       <c r="J91" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
@@ -11856,10 +11863,10 @@
         <v>129</v>
       </c>
       <c r="I92" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J92" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
@@ -11873,10 +11880,10 @@
         <v>129</v>
       </c>
       <c r="I93" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J93" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
@@ -11890,10 +11897,10 @@
         <v>129</v>
       </c>
       <c r="I94" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J94" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
@@ -11907,10 +11914,10 @@
         <v>129</v>
       </c>
       <c r="I95" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J95" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
@@ -11927,7 +11934,7 @@
         <v>132</v>
       </c>
       <c r="J96" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="97" spans="6:10" x14ac:dyDescent="0.3">
@@ -11944,7 +11951,7 @@
         <v>133</v>
       </c>
       <c r="J97" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="98" spans="6:10" x14ac:dyDescent="0.3">
@@ -11952,16 +11959,16 @@
         <v>130</v>
       </c>
       <c r="G98" t="s">
+        <v>322</v>
+      </c>
+      <c r="H98" t="s">
+        <v>322</v>
+      </c>
+      <c r="I98" t="s">
         <v>323</v>
       </c>
-      <c r="H98" t="s">
-        <v>323</v>
-      </c>
-      <c r="I98" t="s">
-        <v>324</v>
-      </c>
       <c r="J98" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="99" spans="6:10" x14ac:dyDescent="0.3">
@@ -11969,20 +11976,19 @@
         <v>130</v>
       </c>
       <c r="G99" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H99" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I99" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J99" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added sgsv and primary region to raw data
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\itpgrfa_crop_indicator_code\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11A51C8-0E48-4DE3-A409-9F0242DAAC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88131515-B3C0-4C66-81DA-356E211AC29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2389" uniqueCount="384">
   <si>
     <t>url</t>
   </si>
@@ -1153,6 +1153,45 @@
   </si>
   <si>
     <t>Reporting_year_endyear</t>
+  </si>
+  <si>
+    <t>genebank_file</t>
+  </si>
+  <si>
+    <t>upov_file</t>
+  </si>
+  <si>
+    <t>gbif_research_file</t>
+  </si>
+  <si>
+    <t>fao_years</t>
+  </si>
+  <si>
+    <t>sgsv_file</t>
+  </si>
+  <si>
+    <t>sgsv_fields</t>
+  </si>
+  <si>
+    <t>accessions_sgsv.csv</t>
+  </si>
+  <si>
+    <t>genus_accessions_sgsv,species_accessions_sgsv</t>
+  </si>
+  <si>
+    <t>sgsv</t>
+  </si>
+  <si>
+    <t>primary_region_file</t>
+  </si>
+  <si>
+    <t>primary_region_fields</t>
+  </si>
+  <si>
+    <t>genus_accessions_primaryregion,species_accessions_primaryregion</t>
+  </si>
+  <si>
+    <t>accessions_primaryregion.csv</t>
   </si>
 </sst>
 </file>
@@ -1516,10 +1555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811487A-6E7B-4C2E-9752-10E8FCDC87C8}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1594,247 +1633,311 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>237</v>
-      </c>
-      <c r="B9" t="s">
-        <v>239</v>
+        <v>374</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B12" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>245</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
+      </c>
+      <c r="B13" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>247</v>
-      </c>
-      <c r="B14" t="s">
-        <v>248</v>
+        <v>245</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>249</v>
-      </c>
-      <c r="B15">
-        <v>2019</v>
+        <v>247</v>
+      </c>
+      <c r="B15" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>250</v>
-      </c>
-      <c r="B16" t="s">
-        <v>251</v>
+        <v>249</v>
+      </c>
+      <c r="B16">
+        <v>2019</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>252</v>
+        <v>371</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>364</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B18" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>255</v>
+        <v>372</v>
       </c>
       <c r="B19" t="s">
-        <v>256</v>
+        <v>362</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B20" t="s">
-        <v>258</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>263</v>
+        <v>373</v>
       </c>
       <c r="B21" t="s">
-        <v>260</v>
+        <v>366</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B22" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>261</v>
+        <v>375</v>
       </c>
       <c r="B23" t="s">
-        <v>262</v>
+        <v>377</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>265</v>
+        <v>376</v>
       </c>
       <c r="B24" t="s">
-        <v>266</v>
+        <v>378</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>267</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>270</v>
+        <v>380</v>
+      </c>
+      <c r="B25" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>268</v>
+        <v>381</v>
       </c>
       <c r="B26" t="s">
-        <v>269</v>
+        <v>382</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="B27" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>273</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>274</v>
+        <v>257</v>
+      </c>
+      <c r="B28" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="B29" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>276</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>274</v>
+        <v>264</v>
+      </c>
+      <c r="B30" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="B31" t="s">
-        <v>286</v>
+        <v>262</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="B32" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>280</v>
-      </c>
-      <c r="B33" t="s">
-        <v>288</v>
+        <v>267</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="B34" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="B35" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>282</v>
-      </c>
-      <c r="B36" t="s">
-        <v>370</v>
+        <v>273</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>283</v>
-      </c>
-      <c r="B37" s="2">
-        <v>2019</v>
+        <v>275</v>
+      </c>
+      <c r="B37" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>276</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>278</v>
+      </c>
+      <c r="B39" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>279</v>
+      </c>
+      <c r="B40" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>280</v>
+      </c>
+      <c r="B41" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>281</v>
+      </c>
+      <c r="B42" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>287</v>
+      </c>
+      <c r="B43" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>282</v>
+      </c>
+      <c r="B44" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>283</v>
+      </c>
+      <c r="B45" s="2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>284</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B46" t="s">
         <v>291</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1" xr:uid="{6B12AD9C-3007-469C-B4F5-178135E8E695}"/>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{6B12AD9C-3007-469C-B4F5-178135E8E695}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1846,7 +1949,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1914,9 +2017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5999D9A-B887-407B-9ED8-3246786298CD}">
   <dimension ref="A1:O161"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -9342,8 +9443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2D5B62-00C5-4824-8379-4A4BEE02241D}">
   <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G95" sqref="G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11921,6 +12022,21 @@
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>379</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C96" t="s">
+        <v>336</v>
+      </c>
+      <c r="D96" t="s">
+        <v>377</v>
+      </c>
+      <c r="E96" t="s">
+        <v>132</v>
+      </c>
       <c r="F96" t="s">
         <v>130</v>
       </c>
@@ -11937,7 +12053,22 @@
         <v>328</v>
       </c>
     </row>
-    <row r="97" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>379</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C97" t="s">
+        <v>336</v>
+      </c>
+      <c r="D97" t="s">
+        <v>377</v>
+      </c>
+      <c r="E97" t="s">
+        <v>133</v>
+      </c>
       <c r="F97" t="s">
         <v>130</v>
       </c>
@@ -11954,7 +12085,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="98" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F98" t="s">
         <v>130</v>
       </c>
@@ -11971,7 +12102,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="99" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F99" t="s">
         <v>130</v>
       </c>

</xml_diff>

<commit_message>
added collection class for processing fao varietal and botanic data
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\itpgrfa_crop_indicator_code\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88131515-B3C0-4C66-81DA-356E211AC29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60742385-F53D-4BB7-A57C-9D815956960B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2389" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2420" uniqueCount="405">
   <si>
     <t>url</t>
   </si>
@@ -1192,6 +1192,69 @@
   </si>
   <si>
     <t>accessions_primaryregion.csv</t>
+  </si>
+  <si>
+    <t>primary_region</t>
+  </si>
+  <si>
+    <t>botanic_file</t>
+  </si>
+  <si>
+    <t>botanic_sheet</t>
+  </si>
+  <si>
+    <t>PlantSearch_2021_7.xlsx</t>
+  </si>
+  <si>
+    <t>PlantSearch metric data</t>
+  </si>
+  <si>
+    <t>Count of institutions</t>
+  </si>
+  <si>
+    <t>botanic_field_genus</t>
+  </si>
+  <si>
+    <t>botanic_field_taxon</t>
+  </si>
+  <si>
+    <t>Genus</t>
+  </si>
+  <si>
+    <t>Taxon</t>
+  </si>
+  <si>
+    <t>botanic_year</t>
+  </si>
+  <si>
+    <t>botanic_fields</t>
+  </si>
+  <si>
+    <t>Wiews_Indicator_40_varietiesreleased_2022_5_12.xlsx</t>
+  </si>
+  <si>
+    <t>fao_varietal_file</t>
+  </si>
+  <si>
+    <t>fao_varietal_sheet</t>
+  </si>
+  <si>
+    <t>fao_varietal_field_genus</t>
+  </si>
+  <si>
+    <t>fao_varietal_field_taxon</t>
+  </si>
+  <si>
+    <t>fao_varietal_year_column</t>
+  </si>
+  <si>
+    <t>YearRelease</t>
+  </si>
+  <si>
+    <t>Taxon_cleaned</t>
+  </si>
+  <si>
+    <t>2015 - 2019 releases</t>
   </si>
 </sst>
 </file>
@@ -1555,10 +1618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811487A-6E7B-4C2E-9752-10E8FCDC87C8}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1933,6 +1996,94 @@
       </c>
       <c r="B46" t="s">
         <v>291</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>385</v>
+      </c>
+      <c r="B47" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>386</v>
+      </c>
+      <c r="B48" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>395</v>
+      </c>
+      <c r="B49" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>390</v>
+      </c>
+      <c r="B50" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>391</v>
+      </c>
+      <c r="B51" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>394</v>
+      </c>
+      <c r="B52">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>397</v>
+      </c>
+      <c r="B53" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>398</v>
+      </c>
+      <c r="B54" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>399</v>
+      </c>
+      <c r="B55" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>400</v>
+      </c>
+      <c r="B56" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>401</v>
+      </c>
+      <c r="B57" t="s">
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -9444,7 +9595,7 @@
   <dimension ref="A1:K99"/>
   <sheetViews>
     <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G95" sqref="G95"/>
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11839,6 +11990,21 @@
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>384</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C87" t="s">
+        <v>336</v>
+      </c>
+      <c r="D87" t="s">
+        <v>383</v>
+      </c>
+      <c r="E87" t="s">
+        <v>127</v>
+      </c>
       <c r="F87" t="s">
         <v>104</v>
       </c>
@@ -11856,6 +12022,21 @@
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>384</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C88" t="s">
+        <v>336</v>
+      </c>
+      <c r="D88" t="s">
+        <v>383</v>
+      </c>
+      <c r="E88" t="s">
+        <v>128</v>
+      </c>
       <c r="F88" t="s">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
added calculate slope for fao data. added calculate indicator in final step
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\itpgrfa_crop_indicator_code\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33441CC9-F577-434C-8855-746F4B351BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5133E1-5FB0-4C0B-96A8-3D8490CC1F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="indicator" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">indicator!$A$1:$J$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">indicator!$A$1:$J$100</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2456" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2640" uniqueCount="435">
   <si>
     <t>url</t>
   </si>
@@ -1008,15 +1008,6 @@
     <t>digital_sequence_supply_gene</t>
   </si>
   <si>
-    <t>backup_genebank_accessions</t>
-  </si>
-  <si>
-    <t>genus_backup_genebank_accessions</t>
-  </si>
-  <si>
-    <t>species_backup_genebank_accessions</t>
-  </si>
-  <si>
     <t>08</t>
   </si>
   <si>
@@ -1146,9 +1137,6 @@
     <t>13</t>
   </si>
   <si>
-    <t>fill_zero</t>
-  </si>
-  <si>
     <t>Trade_Crops_Livestock_E_All_Data.csv</t>
   </si>
   <si>
@@ -1312,6 +1300,51 @@
   </si>
   <si>
     <t>ncbi_year</t>
+  </si>
+  <si>
+    <t>indicator_method</t>
+  </si>
+  <si>
+    <t>across_crops</t>
+  </si>
+  <si>
+    <t>by_value</t>
+  </si>
+  <si>
+    <t>indicator_value</t>
+  </si>
+  <si>
+    <t>pubmed_central</t>
+  </si>
+  <si>
+    <t>pubmed_taxon</t>
+  </si>
+  <si>
+    <t>ncbi</t>
+  </si>
+  <si>
+    <t>ncbi.csv</t>
+  </si>
+  <si>
+    <t>pmc</t>
+  </si>
+  <si>
+    <t>nuccore</t>
+  </si>
+  <si>
+    <t>protein</t>
+  </si>
+  <si>
+    <t>genome</t>
+  </si>
+  <si>
+    <t>gene</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -1335,12 +1368,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1356,10 +1395,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1677,7 +1718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811487A-6E7B-4C2E-9752-10E8FCDC87C8}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
@@ -1753,7 +1794,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>270</v>
@@ -1817,10 +1858,10 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B17" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -1833,10 +1874,10 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B19" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1849,10 +1890,10 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B21" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -1865,34 +1906,34 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B23" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B24" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B25" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B26" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -2036,7 +2077,7 @@
         <v>282</v>
       </c>
       <c r="B44" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -2057,47 +2098,47 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B47" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B48" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B49" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B50" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B51" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B52">
         <v>2022</v>
@@ -2105,71 +2146,71 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B53" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B54" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B55" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B56" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="B57" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B59" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="B60" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B61">
         <v>2022</v>
@@ -9682,10 +9723,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2D5B62-00C5-4824-8379-4A4BEE02241D}">
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E94" sqref="A94:E97"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9700,9 +9741,10 @@
     <col min="8" max="8" width="40.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>292</v>
       </c>
@@ -9731,18 +9773,21 @@
         <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="K1" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>420</v>
+      </c>
+      <c r="L1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>222</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C2" t="s">
         <v>302</v>
@@ -9766,15 +9811,18 @@
         <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>222</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C3" t="s">
         <v>302</v>
@@ -9798,15 +9846,18 @@
         <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>222</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C4" t="s">
         <v>302</v>
@@ -9830,15 +9881,18 @@
         <v>25</v>
       </c>
       <c r="J4" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K4" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>222</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C5" t="s">
         <v>302</v>
@@ -9862,15 +9916,18 @@
         <v>26</v>
       </c>
       <c r="J5" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>222</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C6" t="s">
         <v>302</v>
@@ -9894,15 +9951,18 @@
         <v>28</v>
       </c>
       <c r="J6" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>222</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C7" t="s">
         <v>302</v>
@@ -9926,15 +9986,18 @@
         <v>30</v>
       </c>
       <c r="J7" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K7" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>222</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C8" t="s">
         <v>302</v>
@@ -9958,21 +10021,24 @@
         <v>32</v>
       </c>
       <c r="J8" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K8" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>222</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C9" t="s">
         <v>302</v>
       </c>
       <c r="D9" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E9" t="s">
         <v>308</v>
@@ -9990,21 +10056,24 @@
         <v>35</v>
       </c>
       <c r="J9" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K9" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>222</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C10" t="s">
         <v>302</v>
       </c>
       <c r="D10" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E10" t="s">
         <v>309</v>
@@ -10022,21 +10091,24 @@
         <v>36</v>
       </c>
       <c r="J10" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K10" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>222</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C11" t="s">
         <v>302</v>
       </c>
       <c r="D11" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E11" t="s">
         <v>310</v>
@@ -10054,21 +10126,24 @@
         <v>38</v>
       </c>
       <c r="J11" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K11" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>222</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C12" t="s">
         <v>302</v>
       </c>
       <c r="D12" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E12" t="s">
         <v>311</v>
@@ -10086,15 +10161,18 @@
         <v>39</v>
       </c>
       <c r="J12" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K12" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>222</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C13" t="s">
         <v>302</v>
@@ -10117,13 +10195,19 @@
       <c r="I13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K13" t="s">
+        <v>422</v>
+      </c>
+      <c r="L13">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>222</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C14" t="s">
         <v>302</v>
@@ -10146,13 +10230,19 @@
       <c r="I14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K14" t="s">
+        <v>422</v>
+      </c>
+      <c r="L14">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>222</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C15" t="s">
         <v>302</v>
@@ -10175,13 +10265,19 @@
       <c r="I15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K15" t="s">
+        <v>422</v>
+      </c>
+      <c r="L15">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>222</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C16" t="s">
         <v>302</v>
@@ -10204,13 +10300,19 @@
       <c r="I16" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" t="s">
+        <v>422</v>
+      </c>
+      <c r="L16">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>222</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C17" t="s">
         <v>302</v>
@@ -10233,13 +10335,19 @@
       <c r="I17" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" t="s">
+        <v>422</v>
+      </c>
+      <c r="L17">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>222</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C18" t="s">
         <v>302</v>
@@ -10262,13 +10370,19 @@
       <c r="I18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18" t="s">
+        <v>422</v>
+      </c>
+      <c r="L18">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>222</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C19" t="s">
         <v>302</v>
@@ -10291,19 +10405,25 @@
       <c r="I19" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" t="s">
+        <v>422</v>
+      </c>
+      <c r="L19">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>222</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C20" t="s">
         <v>302</v>
       </c>
       <c r="D20" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E20" t="s">
         <v>308</v>
@@ -10320,19 +10440,25 @@
       <c r="I20" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20" t="s">
+        <v>422</v>
+      </c>
+      <c r="L20">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>222</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C21" t="s">
         <v>302</v>
       </c>
       <c r="D21" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E21" t="s">
         <v>309</v>
@@ -10349,19 +10475,25 @@
       <c r="I21" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" t="s">
+        <v>422</v>
+      </c>
+      <c r="L21">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>222</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C22" t="s">
         <v>302</v>
       </c>
       <c r="D22" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E22" t="s">
         <v>310</v>
@@ -10378,19 +10510,25 @@
       <c r="I22" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22" t="s">
+        <v>422</v>
+      </c>
+      <c r="L22">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>222</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C23" t="s">
         <v>302</v>
       </c>
       <c r="D23" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E23" t="s">
         <v>311</v>
@@ -10407,13 +10545,19 @@
       <c r="I23" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K23" t="s">
+        <v>422</v>
+      </c>
+      <c r="L23">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>222</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C24" t="s">
         <v>302</v>
@@ -10437,15 +10581,15 @@
         <v>19</v>
       </c>
       <c r="J24" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>222</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C25" t="s">
         <v>302</v>
@@ -10469,15 +10613,15 @@
         <v>23</v>
       </c>
       <c r="J25" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>222</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C26" t="s">
         <v>302</v>
@@ -10501,15 +10645,15 @@
         <v>25</v>
       </c>
       <c r="J26" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>222</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C27" t="s">
         <v>302</v>
@@ -10533,15 +10677,15 @@
         <v>26</v>
       </c>
       <c r="J27" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>222</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C28" t="s">
         <v>302</v>
@@ -10565,15 +10709,15 @@
         <v>28</v>
       </c>
       <c r="J28" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>222</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C29" t="s">
         <v>302</v>
@@ -10597,15 +10741,15 @@
         <v>30</v>
       </c>
       <c r="J29" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>222</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C30" t="s">
         <v>302</v>
@@ -10629,21 +10773,21 @@
         <v>32</v>
       </c>
       <c r="J30" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>222</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C31" t="s">
         <v>302</v>
       </c>
       <c r="D31" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E31" t="s">
         <v>308</v>
@@ -10661,21 +10805,21 @@
         <v>35</v>
       </c>
       <c r="J31" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>222</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C32" t="s">
         <v>302</v>
       </c>
       <c r="D32" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E32" t="s">
         <v>309</v>
@@ -10693,21 +10837,21 @@
         <v>36</v>
       </c>
       <c r="J32" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>222</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C33" t="s">
         <v>302</v>
       </c>
       <c r="D33" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E33" t="s">
         <v>310</v>
@@ -10725,21 +10869,21 @@
         <v>38</v>
       </c>
       <c r="J33" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>222</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C34" t="s">
         <v>302</v>
       </c>
       <c r="D34" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E34" t="s">
         <v>311</v>
@@ -10757,10 +10901,25 @@
         <v>39</v>
       </c>
       <c r="J34" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>222</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C35" t="s">
+        <v>302</v>
+      </c>
+      <c r="D35" t="s">
+        <v>304</v>
+      </c>
+      <c r="E35" t="s">
+        <v>303</v>
+      </c>
       <c r="F35" t="s">
         <v>16</v>
       </c>
@@ -10774,10 +10933,25 @@
         <v>19</v>
       </c>
       <c r="J35" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>222</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C36" t="s">
+        <v>302</v>
+      </c>
+      <c r="D36" t="s">
+        <v>304</v>
+      </c>
+      <c r="E36" t="s">
+        <v>305</v>
+      </c>
       <c r="F36" t="s">
         <v>16</v>
       </c>
@@ -10791,10 +10965,25 @@
         <v>23</v>
       </c>
       <c r="J36" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>222</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C37" t="s">
+        <v>302</v>
+      </c>
+      <c r="D37" t="s">
+        <v>304</v>
+      </c>
+      <c r="E37" t="s">
+        <v>306</v>
+      </c>
       <c r="F37" t="s">
         <v>16</v>
       </c>
@@ -10808,10 +10997,25 @@
         <v>25</v>
       </c>
       <c r="J37" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>222</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C38" t="s">
+        <v>302</v>
+      </c>
+      <c r="D38" t="s">
+        <v>304</v>
+      </c>
+      <c r="E38" t="s">
+        <v>307</v>
+      </c>
       <c r="F38" t="s">
         <v>16</v>
       </c>
@@ -10825,10 +11029,25 @@
         <v>26</v>
       </c>
       <c r="J38" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>222</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C39" t="s">
+        <v>302</v>
+      </c>
+      <c r="D39" t="s">
+        <v>297</v>
+      </c>
+      <c r="E39" t="s">
+        <v>298</v>
+      </c>
       <c r="F39" t="s">
         <v>16</v>
       </c>
@@ -10842,10 +11061,25 @@
         <v>28</v>
       </c>
       <c r="J39" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>222</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C40" t="s">
+        <v>302</v>
+      </c>
+      <c r="D40" t="s">
+        <v>297</v>
+      </c>
+      <c r="E40" t="s">
+        <v>229</v>
+      </c>
       <c r="F40" t="s">
         <v>16</v>
       </c>
@@ -10859,10 +11093,25 @@
         <v>30</v>
       </c>
       <c r="J40" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>222</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C41" t="s">
+        <v>302</v>
+      </c>
+      <c r="D41" t="s">
+        <v>300</v>
+      </c>
+      <c r="E41" t="s">
+        <v>299</v>
+      </c>
       <c r="F41" t="s">
         <v>16</v>
       </c>
@@ -10876,10 +11125,25 @@
         <v>32</v>
       </c>
       <c r="J41" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>222</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C42" t="s">
+        <v>302</v>
+      </c>
+      <c r="D42" t="s">
+        <v>365</v>
+      </c>
+      <c r="E42" t="s">
+        <v>308</v>
+      </c>
       <c r="F42" t="s">
         <v>16</v>
       </c>
@@ -10893,10 +11157,25 @@
         <v>35</v>
       </c>
       <c r="J42" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>222</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C43" t="s">
+        <v>302</v>
+      </c>
+      <c r="D43" t="s">
+        <v>365</v>
+      </c>
+      <c r="E43" t="s">
+        <v>309</v>
+      </c>
       <c r="F43" t="s">
         <v>16</v>
       </c>
@@ -10910,10 +11189,25 @@
         <v>36</v>
       </c>
       <c r="J43" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>222</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C44" t="s">
+        <v>302</v>
+      </c>
+      <c r="D44" t="s">
+        <v>365</v>
+      </c>
+      <c r="E44" t="s">
+        <v>310</v>
+      </c>
       <c r="F44" t="s">
         <v>16</v>
       </c>
@@ -10927,10 +11221,25 @@
         <v>38</v>
       </c>
       <c r="J44" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>222</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C45" t="s">
+        <v>302</v>
+      </c>
+      <c r="D45" t="s">
+        <v>365</v>
+      </c>
+      <c r="E45" t="s">
+        <v>311</v>
+      </c>
       <c r="F45" t="s">
         <v>16</v>
       </c>
@@ -10944,24 +11253,24 @@
         <v>39</v>
       </c>
       <c r="J45" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C46" t="s">
         <v>302</v>
       </c>
       <c r="D46" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="E46" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="F46" t="s">
         <v>16</v>
@@ -10976,24 +11285,27 @@
         <v>70</v>
       </c>
       <c r="J46" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K46" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C47" t="s">
         <v>302</v>
       </c>
       <c r="D47" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="E47" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F47" t="s">
         <v>16</v>
@@ -11008,24 +11320,27 @@
         <v>71</v>
       </c>
       <c r="J47" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K47" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C48" t="s">
         <v>302</v>
       </c>
       <c r="D48" t="s">
+        <v>328</v>
+      </c>
+      <c r="E48" t="s">
         <v>331</v>
-      </c>
-      <c r="E48" t="s">
-        <v>334</v>
       </c>
       <c r="F48" t="s">
         <v>16</v>
@@ -11040,56 +11355,62 @@
         <v>72</v>
       </c>
       <c r="J48" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K48" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>335</v>
+        <v>426</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C49" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D49" t="s">
-        <v>337</v>
+        <v>427</v>
       </c>
       <c r="E49" t="s">
-        <v>339</v>
+        <v>428</v>
       </c>
       <c r="F49" t="s">
         <v>16</v>
       </c>
       <c r="G49" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H49" t="s">
-        <v>74</v>
+        <v>424</v>
       </c>
       <c r="I49" t="s">
-        <v>70</v>
+        <v>425</v>
       </c>
       <c r="J49" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K49" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C50" t="s">
+        <v>333</v>
+      </c>
+      <c r="D50" t="s">
+        <v>334</v>
+      </c>
+      <c r="E50" t="s">
         <v>336</v>
-      </c>
-      <c r="D50" t="s">
-        <v>337</v>
-      </c>
-      <c r="E50" t="s">
-        <v>338</v>
       </c>
       <c r="F50" t="s">
         <v>16</v>
@@ -11101,27 +11422,30 @@
         <v>74</v>
       </c>
       <c r="I50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J50" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K50" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>332</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C51" t="s">
+        <v>333</v>
+      </c>
+      <c r="D51" t="s">
+        <v>334</v>
+      </c>
+      <c r="E51" t="s">
         <v>335</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C51" t="s">
-        <v>336</v>
-      </c>
-      <c r="D51" t="s">
-        <v>337</v>
-      </c>
-      <c r="E51" t="s">
-        <v>340</v>
       </c>
       <c r="F51" t="s">
         <v>16</v>
@@ -11133,50 +11457,56 @@
         <v>74</v>
       </c>
       <c r="I51" t="s">
+        <v>71</v>
+      </c>
+      <c r="J51" t="s">
+        <v>325</v>
+      </c>
+      <c r="K51" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>332</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C52" t="s">
+        <v>333</v>
+      </c>
+      <c r="D52" t="s">
+        <v>334</v>
+      </c>
+      <c r="E52" t="s">
+        <v>337</v>
+      </c>
+      <c r="F52" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" t="s">
+        <v>73</v>
+      </c>
+      <c r="H52" t="s">
+        <v>74</v>
+      </c>
+      <c r="I52" t="s">
         <v>72</v>
       </c>
-      <c r="J51" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>222</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="C52" t="s">
-        <v>302</v>
-      </c>
-      <c r="D52" t="s">
-        <v>304</v>
-      </c>
-      <c r="E52" t="s">
-        <v>303</v>
-      </c>
-      <c r="F52" t="s">
-        <v>75</v>
-      </c>
-      <c r="G52" t="s">
-        <v>17</v>
-      </c>
-      <c r="H52" t="s">
-        <v>18</v>
-      </c>
-      <c r="I52" t="s">
-        <v>76</v>
-      </c>
       <c r="J52" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K52" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>222</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C53" t="s">
         <v>302</v>
@@ -11185,7 +11515,7 @@
         <v>304</v>
       </c>
       <c r="E53" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F53" t="s">
         <v>75</v>
@@ -11197,18 +11527,18 @@
         <v>18</v>
       </c>
       <c r="I53" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J53" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>222</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C54" t="s">
         <v>302</v>
@@ -11217,7 +11547,7 @@
         <v>304</v>
       </c>
       <c r="E54" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F54" t="s">
         <v>75</v>
@@ -11229,18 +11559,18 @@
         <v>18</v>
       </c>
       <c r="I54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J54" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>222</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C55" t="s">
         <v>302</v>
@@ -11249,7 +11579,7 @@
         <v>304</v>
       </c>
       <c r="E55" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F55" t="s">
         <v>75</v>
@@ -11261,27 +11591,27 @@
         <v>18</v>
       </c>
       <c r="I55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J55" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>222</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C56" t="s">
         <v>302</v>
       </c>
       <c r="D56" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="E56" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="F56" t="s">
         <v>75</v>
@@ -11290,21 +11620,21 @@
         <v>17</v>
       </c>
       <c r="H56" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="I56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J56" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>222</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C57" t="s">
         <v>302</v>
@@ -11313,7 +11643,7 @@
         <v>297</v>
       </c>
       <c r="E57" t="s">
-        <v>229</v>
+        <v>298</v>
       </c>
       <c r="F57" t="s">
         <v>75</v>
@@ -11325,27 +11655,27 @@
         <v>27</v>
       </c>
       <c r="I57" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J57" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>222</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C58" t="s">
         <v>302</v>
       </c>
       <c r="D58" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E58" t="s">
-        <v>299</v>
+        <v>229</v>
       </c>
       <c r="F58" t="s">
         <v>75</v>
@@ -11357,27 +11687,27 @@
         <v>27</v>
       </c>
       <c r="I58" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J58" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>222</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C59" t="s">
         <v>302</v>
       </c>
       <c r="D59" t="s">
-        <v>369</v>
+        <v>300</v>
       </c>
       <c r="E59" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="F59" t="s">
         <v>75</v>
@@ -11386,30 +11716,30 @@
         <v>17</v>
       </c>
       <c r="H59" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="I59" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J59" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>222</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C60" t="s">
         <v>302</v>
       </c>
       <c r="D60" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E60" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F60" t="s">
         <v>75</v>
@@ -11421,27 +11751,27 @@
         <v>34</v>
       </c>
       <c r="I60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J60" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>222</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C61" t="s">
         <v>302</v>
       </c>
       <c r="D61" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E61" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F61" t="s">
         <v>75</v>
@@ -11453,27 +11783,27 @@
         <v>34</v>
       </c>
       <c r="I61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J61" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>222</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C62" t="s">
         <v>302</v>
       </c>
       <c r="D62" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E62" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F62" t="s">
         <v>75</v>
@@ -11485,30 +11815,60 @@
         <v>34</v>
       </c>
       <c r="I62" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J62" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>222</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C63" t="s">
+        <v>302</v>
+      </c>
+      <c r="D63" t="s">
+        <v>365</v>
+      </c>
+      <c r="E63" t="s">
+        <v>311</v>
+      </c>
       <c r="F63" t="s">
         <v>75</v>
       </c>
       <c r="G63" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="H63" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="I63" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="J63" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>222</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C64" t="s">
+        <v>302</v>
+      </c>
+      <c r="D64" t="s">
+        <v>304</v>
+      </c>
+      <c r="E64" t="s">
+        <v>303</v>
+      </c>
       <c r="F64" t="s">
         <v>75</v>
       </c>
@@ -11519,13 +11879,28 @@
         <v>18</v>
       </c>
       <c r="I64" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J64" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>222</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C65" t="s">
+        <v>302</v>
+      </c>
+      <c r="D65" t="s">
+        <v>304</v>
+      </c>
+      <c r="E65" t="s">
+        <v>305</v>
+      </c>
       <c r="F65" t="s">
         <v>75</v>
       </c>
@@ -11536,13 +11911,28 @@
         <v>18</v>
       </c>
       <c r="I65" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J65" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>222</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C66" t="s">
+        <v>302</v>
+      </c>
+      <c r="D66" t="s">
+        <v>304</v>
+      </c>
+      <c r="E66" t="s">
+        <v>306</v>
+      </c>
       <c r="F66" t="s">
         <v>75</v>
       </c>
@@ -11553,13 +11943,28 @@
         <v>18</v>
       </c>
       <c r="I66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J66" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>222</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C67" t="s">
+        <v>302</v>
+      </c>
+      <c r="D67" t="s">
+        <v>304</v>
+      </c>
+      <c r="E67" t="s">
+        <v>307</v>
+      </c>
       <c r="F67" t="s">
         <v>75</v>
       </c>
@@ -11567,16 +11972,31 @@
         <v>52</v>
       </c>
       <c r="H67" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="I67" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J67" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>222</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C68" t="s">
+        <v>302</v>
+      </c>
+      <c r="D68" t="s">
+        <v>297</v>
+      </c>
+      <c r="E68" t="s">
+        <v>298</v>
+      </c>
       <c r="F68" t="s">
         <v>75</v>
       </c>
@@ -11587,13 +12007,28 @@
         <v>27</v>
       </c>
       <c r="I68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J68" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>222</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C69" t="s">
+        <v>302</v>
+      </c>
+      <c r="D69" t="s">
+        <v>297</v>
+      </c>
+      <c r="E69" t="s">
+        <v>229</v>
+      </c>
       <c r="F69" t="s">
         <v>75</v>
       </c>
@@ -11604,13 +12039,28 @@
         <v>27</v>
       </c>
       <c r="I69" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J69" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>222</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C70" t="s">
+        <v>302</v>
+      </c>
+      <c r="D70" t="s">
+        <v>300</v>
+      </c>
+      <c r="E70" t="s">
+        <v>299</v>
+      </c>
       <c r="F70" t="s">
         <v>75</v>
       </c>
@@ -11618,16 +12068,31 @@
         <v>52</v>
       </c>
       <c r="H70" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="I70" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J70" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>222</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C71" t="s">
+        <v>302</v>
+      </c>
+      <c r="D71" t="s">
+        <v>365</v>
+      </c>
+      <c r="E71" t="s">
+        <v>308</v>
+      </c>
       <c r="F71" t="s">
         <v>75</v>
       </c>
@@ -11638,13 +12103,28 @@
         <v>34</v>
       </c>
       <c r="I71" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J71" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>222</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C72" t="s">
+        <v>302</v>
+      </c>
+      <c r="D72" t="s">
+        <v>365</v>
+      </c>
+      <c r="E72" t="s">
+        <v>309</v>
+      </c>
       <c r="F72" t="s">
         <v>75</v>
       </c>
@@ -11655,13 +12135,28 @@
         <v>34</v>
       </c>
       <c r="I72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J72" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>222</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C73" t="s">
+        <v>302</v>
+      </c>
+      <c r="D73" t="s">
+        <v>365</v>
+      </c>
+      <c r="E73" t="s">
+        <v>310</v>
+      </c>
       <c r="F73" t="s">
         <v>75</v>
       </c>
@@ -11672,47 +12167,47 @@
         <v>34</v>
       </c>
       <c r="I73" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J73" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>354</v>
+        <v>222</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>360</v>
+        <v>434</v>
       </c>
       <c r="C74" t="s">
         <v>302</v>
       </c>
       <c r="D74" t="s">
-        <v>256</v>
+        <v>365</v>
       </c>
       <c r="E74" t="s">
-        <v>359</v>
+        <v>311</v>
       </c>
       <c r="F74" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="G74" t="s">
-        <v>312</v>
+        <v>52</v>
       </c>
       <c r="H74" t="s">
-        <v>312</v>
+        <v>34</v>
       </c>
       <c r="I74" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="J74" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>357</v>
@@ -11724,30 +12219,33 @@
         <v>256</v>
       </c>
       <c r="E75" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F75" t="s">
         <v>88</v>
       </c>
       <c r="G75" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H75" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I75" t="s">
-        <v>314</v>
+        <v>93</v>
       </c>
       <c r="J75" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K75" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>351</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>354</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>355</v>
       </c>
       <c r="C76" t="s">
         <v>302</v>
@@ -11756,71 +12254,77 @@
         <v>256</v>
       </c>
       <c r="E76" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F76" t="s">
         <v>88</v>
       </c>
       <c r="G76" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H76" t="s">
-        <v>95</v>
+        <v>314</v>
       </c>
       <c r="I76" t="s">
-        <v>96</v>
+        <v>314</v>
       </c>
       <c r="J76" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K76" t="s">
+        <v>422</v>
+      </c>
+      <c r="L76">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>330</v>
+        <v>352</v>
       </c>
       <c r="C77" t="s">
         <v>302</v>
       </c>
       <c r="D77" t="s">
-        <v>351</v>
+        <v>256</v>
       </c>
       <c r="E77" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F77" t="s">
         <v>88</v>
       </c>
       <c r="G77" t="s">
-        <v>90</v>
+        <v>315</v>
       </c>
       <c r="H77" t="s">
-        <v>316</v>
+        <v>95</v>
       </c>
       <c r="I77" t="s">
-        <v>316</v>
+        <v>96</v>
       </c>
       <c r="J77" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C78" t="s">
         <v>302</v>
       </c>
       <c r="D78" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E78" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="F78" t="s">
         <v>88</v>
@@ -11829,59 +12333,68 @@
         <v>90</v>
       </c>
       <c r="H78" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I78" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J78" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K78" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>409</v>
+        <v>347</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C79" t="s">
         <v>302</v>
       </c>
       <c r="D79" t="s">
-        <v>410</v>
+        <v>348</v>
       </c>
       <c r="E79" t="s">
-        <v>411</v>
+        <v>350</v>
       </c>
       <c r="F79" t="s">
         <v>88</v>
       </c>
       <c r="G79" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="H79" t="s">
-        <v>98</v>
+        <v>317</v>
       </c>
       <c r="I79" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+      <c r="J79" t="s">
+        <v>325</v>
+      </c>
+      <c r="K79" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C80" t="s">
         <v>302</v>
       </c>
       <c r="D80" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="E80" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="F80" t="s">
         <v>88</v>
@@ -11893,91 +12406,100 @@
         <v>98</v>
       </c>
       <c r="I80" t="s">
+        <v>403</v>
+      </c>
+      <c r="J80" t="s">
+        <v>325</v>
+      </c>
+      <c r="K80" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>405</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C81" t="s">
+        <v>302</v>
+      </c>
+      <c r="D81" t="s">
+        <v>406</v>
+      </c>
+      <c r="E81" t="s">
         <v>408</v>
-      </c>
-      <c r="J80" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>361</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C81" t="s">
-        <v>336</v>
-      </c>
-      <c r="D81" t="s">
-        <v>362</v>
-      </c>
-      <c r="E81" t="s">
-        <v>101</v>
       </c>
       <c r="F81" t="s">
         <v>88</v>
       </c>
       <c r="G81" t="s">
+        <v>98</v>
+      </c>
+      <c r="H81" t="s">
+        <v>98</v>
+      </c>
+      <c r="I81" t="s">
+        <v>404</v>
+      </c>
+      <c r="J81" t="s">
+        <v>325</v>
+      </c>
+      <c r="K81" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>358</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C82" t="s">
+        <v>333</v>
+      </c>
+      <c r="D82" t="s">
+        <v>359</v>
+      </c>
+      <c r="E82" t="s">
+        <v>101</v>
+      </c>
+      <c r="F82" t="s">
+        <v>88</v>
+      </c>
+      <c r="G82" t="s">
         <v>100</v>
       </c>
-      <c r="H81" t="s">
+      <c r="H82" t="s">
         <v>100</v>
       </c>
-      <c r="I81" t="s">
+      <c r="I82" t="s">
         <v>101</v>
       </c>
-      <c r="J81" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>363</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C82" t="s">
-        <v>336</v>
-      </c>
-      <c r="D82" t="s">
-        <v>364</v>
-      </c>
-      <c r="E82" t="s">
+      <c r="J82" t="s">
+        <v>325</v>
+      </c>
+      <c r="K82" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>360</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C83" t="s">
+        <v>333</v>
+      </c>
+      <c r="D83" t="s">
+        <v>361</v>
+      </c>
+      <c r="E83" t="s">
         <v>107</v>
-      </c>
-      <c r="F82" t="s">
-        <v>104</v>
-      </c>
-      <c r="G82" t="s">
-        <v>105</v>
-      </c>
-      <c r="H82" t="s">
-        <v>106</v>
-      </c>
-      <c r="I82" t="s">
-        <v>107</v>
-      </c>
-      <c r="J82" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>363</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C83" t="s">
-        <v>336</v>
-      </c>
-      <c r="D83" t="s">
-        <v>364</v>
-      </c>
-      <c r="E83" t="s">
-        <v>109</v>
       </c>
       <c r="F83" t="s">
         <v>104</v>
@@ -11989,187 +12511,205 @@
         <v>106</v>
       </c>
       <c r="I83" t="s">
+        <v>107</v>
+      </c>
+      <c r="J83" t="s">
+        <v>325</v>
+      </c>
+      <c r="K83" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>360</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C84" t="s">
+        <v>333</v>
+      </c>
+      <c r="D84" t="s">
+        <v>361</v>
+      </c>
+      <c r="E84" t="s">
         <v>109</v>
-      </c>
-      <c r="J83" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>342</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C84" t="s">
-        <v>302</v>
-      </c>
-      <c r="D84" t="s">
-        <v>343</v>
-      </c>
-      <c r="E84" t="s">
-        <v>344</v>
       </c>
       <c r="F84" t="s">
         <v>104</v>
       </c>
       <c r="G84" t="s">
+        <v>105</v>
+      </c>
+      <c r="H84" t="s">
+        <v>106</v>
+      </c>
+      <c r="I84" t="s">
+        <v>109</v>
+      </c>
+      <c r="J84" t="s">
+        <v>325</v>
+      </c>
+      <c r="K84" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G85" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H85" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I85" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J84" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+      <c r="J85" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="K85" s="3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="E86" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C85" t="s">
+      <c r="F86" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="K86" s="3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C87" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D87" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I87" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J87" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="K87" s="3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="E85" t="s">
-        <v>345</v>
-      </c>
-      <c r="F85" t="s">
+      <c r="B88" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="F88" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G88" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H85" t="s">
-        <v>113</v>
-      </c>
-      <c r="I85" t="s">
-        <v>115</v>
-      </c>
-      <c r="J85" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>346</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C86" t="s">
-        <v>302</v>
-      </c>
-      <c r="D86" t="s">
-        <v>347</v>
-      </c>
-      <c r="E86" t="s">
-        <v>348</v>
-      </c>
-      <c r="F86" t="s">
-        <v>104</v>
-      </c>
-      <c r="G86" t="s">
-        <v>111</v>
-      </c>
-      <c r="H86" t="s">
+      <c r="H88" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="I86" t="s">
-        <v>118</v>
-      </c>
-      <c r="J86" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>346</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C87" t="s">
-        <v>302</v>
-      </c>
-      <c r="D87" t="s">
-        <v>347</v>
-      </c>
-      <c r="E87" t="s">
-        <v>349</v>
-      </c>
-      <c r="F87" t="s">
-        <v>104</v>
-      </c>
-      <c r="G87" t="s">
-        <v>111</v>
-      </c>
-      <c r="H87" t="s">
-        <v>117</v>
-      </c>
-      <c r="I87" t="s">
+      <c r="I88" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="J87" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>384</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C88" t="s">
-        <v>336</v>
-      </c>
-      <c r="D88" t="s">
-        <v>383</v>
-      </c>
-      <c r="E88" t="s">
+      <c r="J88" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="K88" s="3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>380</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C89" t="s">
+        <v>333</v>
+      </c>
+      <c r="D89" t="s">
+        <v>379</v>
+      </c>
+      <c r="E89" t="s">
         <v>127</v>
-      </c>
-      <c r="F88" t="s">
-        <v>104</v>
-      </c>
-      <c r="G88" t="s">
-        <v>126</v>
-      </c>
-      <c r="H88" t="s">
-        <v>126</v>
-      </c>
-      <c r="I88" t="s">
-        <v>127</v>
-      </c>
-      <c r="J88" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>384</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C89" t="s">
-        <v>336</v>
-      </c>
-      <c r="D89" t="s">
-        <v>383</v>
-      </c>
-      <c r="E89" t="s">
-        <v>128</v>
       </c>
       <c r="F89" t="s">
         <v>104</v>
@@ -12181,59 +12721,59 @@
         <v>126</v>
       </c>
       <c r="I89" t="s">
+        <v>127</v>
+      </c>
+      <c r="J89" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>380</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C90" t="s">
+        <v>333</v>
+      </c>
+      <c r="D90" t="s">
+        <v>379</v>
+      </c>
+      <c r="E90" t="s">
         <v>128</v>
-      </c>
-      <c r="J89" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>413</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C90" t="s">
-        <v>302</v>
-      </c>
-      <c r="D90" t="s">
-        <v>414</v>
-      </c>
-      <c r="E90" t="s">
-        <v>415</v>
       </c>
       <c r="F90" t="s">
         <v>104</v>
       </c>
       <c r="G90" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H90" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I90" t="s">
-        <v>405</v>
+        <v>128</v>
       </c>
       <c r="J90" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C91" t="s">
         <v>302</v>
       </c>
       <c r="D91" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="E91" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="F91" t="s">
         <v>104</v>
@@ -12245,59 +12785,65 @@
         <v>125</v>
       </c>
       <c r="I91" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="J91" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K91" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>365</v>
+        <v>409</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C92" t="s">
-        <v>336</v>
+        <v>302</v>
       </c>
       <c r="D92" t="s">
-        <v>366</v>
+        <v>410</v>
       </c>
       <c r="E92" t="s">
-        <v>122</v>
+        <v>412</v>
       </c>
       <c r="F92" t="s">
         <v>104</v>
       </c>
       <c r="G92" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="H92" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="I92" t="s">
+        <v>402</v>
+      </c>
+      <c r="J92" t="s">
+        <v>325</v>
+      </c>
+      <c r="K92" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>362</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C93" t="s">
+        <v>333</v>
+      </c>
+      <c r="D93" t="s">
+        <v>363</v>
+      </c>
+      <c r="E93" t="s">
         <v>122</v>
-      </c>
-      <c r="J92" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>365</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C93" t="s">
-        <v>336</v>
-      </c>
-      <c r="D93" t="s">
-        <v>366</v>
-      </c>
-      <c r="E93" t="s">
-        <v>124</v>
       </c>
       <c r="F93" t="s">
         <v>104</v>
@@ -12309,30 +12855,66 @@
         <v>121</v>
       </c>
       <c r="I93" t="s">
+        <v>122</v>
+      </c>
+      <c r="J93" t="s">
+        <v>325</v>
+      </c>
+      <c r="K93" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>362</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C94" t="s">
+        <v>333</v>
+      </c>
+      <c r="D94" t="s">
+        <v>363</v>
+      </c>
+      <c r="E94" t="s">
         <v>124</v>
       </c>
-      <c r="J93" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F94" t="s">
         <v>104</v>
       </c>
       <c r="G94" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="H94" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="I94" t="s">
-        <v>318</v>
+        <v>124</v>
       </c>
       <c r="J94" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K94" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>426</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C95" t="s">
+        <v>333</v>
+      </c>
+      <c r="D95" t="s">
+        <v>427</v>
+      </c>
+      <c r="E95" t="s">
+        <v>429</v>
+      </c>
       <c r="F95" t="s">
         <v>104</v>
       </c>
@@ -12343,13 +12925,31 @@
         <v>129</v>
       </c>
       <c r="I95" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J95" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K95" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>426</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C96" t="s">
+        <v>333</v>
+      </c>
+      <c r="D96" t="s">
+        <v>427</v>
+      </c>
+      <c r="E96" t="s">
+        <v>430</v>
+      </c>
       <c r="F96" t="s">
         <v>104</v>
       </c>
@@ -12360,13 +12960,31 @@
         <v>129</v>
       </c>
       <c r="I96" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J96" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="K96" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>426</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C97" t="s">
+        <v>333</v>
+      </c>
+      <c r="D97" t="s">
+        <v>427</v>
+      </c>
+      <c r="E97" t="s">
+        <v>431</v>
+      </c>
       <c r="F97" t="s">
         <v>104</v>
       </c>
@@ -12377,59 +12995,65 @@
         <v>129</v>
       </c>
       <c r="I97" t="s">
+        <v>320</v>
+      </c>
+      <c r="J97" t="s">
+        <v>325</v>
+      </c>
+      <c r="K97" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>426</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C98" t="s">
+        <v>333</v>
+      </c>
+      <c r="D98" t="s">
+        <v>427</v>
+      </c>
+      <c r="E98" t="s">
+        <v>432</v>
+      </c>
+      <c r="F98" t="s">
+        <v>104</v>
+      </c>
+      <c r="G98" t="s">
+        <v>129</v>
+      </c>
+      <c r="H98" t="s">
+        <v>129</v>
+      </c>
+      <c r="I98" t="s">
         <v>321</v>
       </c>
-      <c r="J97" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>379</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C98" t="s">
-        <v>336</v>
-      </c>
-      <c r="D98" t="s">
-        <v>377</v>
-      </c>
-      <c r="E98" t="s">
+      <c r="J98" t="s">
+        <v>325</v>
+      </c>
+      <c r="K98" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>375</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C99" t="s">
+        <v>333</v>
+      </c>
+      <c r="D99" t="s">
+        <v>373</v>
+      </c>
+      <c r="E99" t="s">
         <v>132</v>
-      </c>
-      <c r="F98" t="s">
-        <v>130</v>
-      </c>
-      <c r="G98" t="s">
-        <v>131</v>
-      </c>
-      <c r="H98" t="s">
-        <v>131</v>
-      </c>
-      <c r="I98" t="s">
-        <v>132</v>
-      </c>
-      <c r="J98" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>379</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C99" t="s">
-        <v>336</v>
-      </c>
-      <c r="D99" t="s">
-        <v>377</v>
-      </c>
-      <c r="E99" t="s">
-        <v>133</v>
       </c>
       <c r="F99" t="s">
         <v>130</v>
@@ -12441,44 +13065,48 @@
         <v>131</v>
       </c>
       <c r="I99" t="s">
+        <v>132</v>
+      </c>
+      <c r="J99" t="s">
+        <v>325</v>
+      </c>
+      <c r="K99" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>375</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C100" t="s">
+        <v>333</v>
+      </c>
+      <c r="D100" t="s">
+        <v>373</v>
+      </c>
+      <c r="E100" t="s">
         <v>133</v>
       </c>
-      <c r="J99" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F100" t="s">
         <v>130</v>
       </c>
       <c r="G100" t="s">
-        <v>322</v>
+        <v>131</v>
       </c>
       <c r="H100" t="s">
-        <v>322</v>
+        <v>131</v>
       </c>
       <c r="I100" t="s">
-        <v>323</v>
+        <v>133</v>
       </c>
       <c r="J100" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F101" t="s">
-        <v>130</v>
-      </c>
-      <c r="G101" t="s">
-        <v>322</v>
-      </c>
-      <c r="H101" t="s">
-        <v>322</v>
-      </c>
-      <c r="I101" t="s">
-        <v>324</v>
-      </c>
-      <c r="J101" t="s">
-        <v>328</v>
+        <v>325</v>
+      </c>
+      <c r="K100" t="s">
+        <v>421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new method for final indicator. fixed slop method for fao
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\itpgrfa_crop_indicator_code\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5133E1-5FB0-4C0B-96A8-3D8490CC1F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A537F07D-4A16-4E75-8472-09AB13B6A895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2640" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2644" uniqueCount="438">
   <si>
     <t>url</t>
   </si>
@@ -1345,6 +1345,15 @@
   </si>
   <si>
     <t>15</t>
+  </si>
+  <si>
+    <t>element_per_crop</t>
+  </si>
+  <si>
+    <t>supply,genebank_collections,origin_country,genus_count_origin_supply</t>
+  </si>
+  <si>
+    <t>supply,genebank_collections,origin_country,species_count_origin_supply</t>
   </si>
 </sst>
 </file>
@@ -9726,7 +9735,7 @@
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10199,7 +10208,7 @@
         <v>422</v>
       </c>
       <c r="L13">
-        <v>237</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -10234,7 +10243,7 @@
         <v>422</v>
       </c>
       <c r="L14">
-        <v>237</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -10269,7 +10278,7 @@
         <v>422</v>
       </c>
       <c r="L15">
-        <v>237</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -10304,7 +10313,7 @@
         <v>422</v>
       </c>
       <c r="L16">
-        <v>237</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -10339,7 +10348,7 @@
         <v>422</v>
       </c>
       <c r="L17">
-        <v>237</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -10374,7 +10383,7 @@
         <v>422</v>
       </c>
       <c r="L18">
-        <v>237</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -10409,7 +10418,7 @@
         <v>422</v>
       </c>
       <c r="L19">
-        <v>237</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -10444,7 +10453,7 @@
         <v>422</v>
       </c>
       <c r="L20">
-        <v>237</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -10479,7 +10488,7 @@
         <v>422</v>
       </c>
       <c r="L21">
-        <v>237</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -10514,7 +10523,7 @@
         <v>422</v>
       </c>
       <c r="L22">
-        <v>237</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -10549,7 +10558,7 @@
         <v>422</v>
       </c>
       <c r="L23">
-        <v>237</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -12275,7 +12284,7 @@
         <v>422</v>
       </c>
       <c r="L76">
-        <v>237</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
@@ -12415,7 +12424,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>405</v>
       </c>
@@ -12450,7 +12459,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>358</v>
       </c>
@@ -12485,7 +12494,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>360</v>
       </c>
@@ -12520,7 +12529,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>360</v>
       </c>
@@ -12555,7 +12564,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="85" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>339</v>
       </c>
@@ -12587,10 +12596,13 @@
         <v>325</v>
       </c>
       <c r="K85" s="3" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>435</v>
+      </c>
+      <c r="L85" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>339</v>
       </c>
@@ -12622,10 +12634,13 @@
         <v>325</v>
       </c>
       <c r="K86" s="3" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>435</v>
+      </c>
+      <c r="L86" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>343</v>
       </c>
@@ -12657,10 +12672,13 @@
         <v>325</v>
       </c>
       <c r="K87" s="3" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>435</v>
+      </c>
+      <c r="L87" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>343</v>
       </c>
@@ -12692,10 +12710,13 @@
         <v>325</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+        <v>435</v>
+      </c>
+      <c r="L88" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>380</v>
       </c>
@@ -12727,7 +12748,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>380</v>
       </c>
@@ -12759,7 +12780,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>409</v>
       </c>
@@ -12794,7 +12815,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>409</v>
       </c>
@@ -12829,7 +12850,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>362</v>
       </c>
@@ -12864,7 +12885,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>362</v>
       </c>
@@ -12899,7 +12920,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>426</v>
       </c>
@@ -12934,7 +12955,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>426</v>
       </c>

</xml_diff>

<commit_message>
fixed conf file with mls data
</commit_message>
<xml_diff>
--- a/data/conf/conf.xlsx
+++ b/data/conf/conf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\CWR\itpgrfa_crop_indicator_code\data\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79D4FD6-9FD2-40CE-8BFB-E3E93B2305F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADB1A9A-7F55-434C-ADF6-D46F6EE6F6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="5" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{E493FFA8-6512-4F94-A4C3-4A5A8E49A981}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4470" uniqueCount="851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4470" uniqueCount="855">
   <si>
     <t>url</t>
   </si>
@@ -2596,6 +2596,18 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>supply,genebank_collections,genebank_collections,genebank_collections_genus</t>
+  </si>
+  <si>
+    <t>supply,genebank_collections,genebank_collections,genebank_collections_taxon</t>
+  </si>
+  <si>
+    <t>mls_accessions_genus</t>
+  </si>
+  <si>
+    <t>mls_accessions_species</t>
   </si>
 </sst>
 </file>
@@ -3571,11 +3583,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2D5B62-00C5-4824-8379-4A4BEE02241D}">
   <dimension ref="A1:L99"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D84" sqref="D84"/>
+      <selection pane="bottomRight" activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6515,7 +6527,7 @@
         <v>337</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>338</v>
+        <v>853</v>
       </c>
       <c r="F84" s="3" t="s">
         <v>104</v>
@@ -6536,7 +6548,7 @@
         <v>432</v>
       </c>
       <c r="L84" s="3" t="s">
-        <v>433</v>
+        <v>851</v>
       </c>
     </row>
     <row r="85" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -6553,7 +6565,7 @@
         <v>337</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>339</v>
+        <v>854</v>
       </c>
       <c r="F85" s="3" t="s">
         <v>104</v>
@@ -6574,7 +6586,7 @@
         <v>432</v>
       </c>
       <c r="L85" s="3" t="s">
-        <v>434</v>
+        <v>852</v>
       </c>
     </row>
     <row r="86" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -6612,7 +6624,7 @@
         <v>432</v>
       </c>
       <c r="L86" s="3" t="s">
-        <v>433</v>
+        <v>851</v>
       </c>
     </row>
     <row r="87" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -6650,7 +6662,7 @@
         <v>432</v>
       </c>
       <c r="L87" s="3" t="s">
-        <v>434</v>
+        <v>852</v>
       </c>
     </row>
     <row r="88" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -17502,7 +17514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05497BFE-A5B8-482B-AEA5-A6788DC9A33B}">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>

</xml_diff>